<commit_message>
Cambios en el ejercicio 1
</commit_message>
<xml_diff>
--- a/resultados_tp5_dinamica.xlsx
+++ b/resultados_tp5_dinamica.xlsx
@@ -472,7 +472,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.999224230787485e-35</v>
+        <v>-1.84450729546213e-17</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +483,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C4" t="n">
-        <v>-9.99844846157497e-35</v>
+        <v>-3.68901459092426e-17</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.499767269236245e-34</v>
+        <v>-5.53352188638639e-17</v>
       </c>
     </row>
     <row r="6">
@@ -505,7 +505,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.999689692314994e-34</v>
+        <v>-7.378029181848519e-17</v>
       </c>
     </row>
     <row r="7">
@@ -516,7 +516,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.499612115393742e-34</v>
+        <v>-9.222536477310648e-17</v>
       </c>
     </row>
     <row r="8">
@@ -527,7 +527,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.99953453847249e-34</v>
+        <v>-1.106704377277278e-16</v>
       </c>
     </row>
     <row r="9">
@@ -538,7 +538,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C9" t="n">
-        <v>-3.499456961551239e-34</v>
+        <v>-1.291155106823491e-16</v>
       </c>
     </row>
     <row r="10">
@@ -549,7 +549,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C10" t="n">
-        <v>-3.999379384629987e-34</v>
+        <v>-1.475605836369704e-16</v>
       </c>
     </row>
     <row r="11">
@@ -560,7 +560,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.499301807708736e-34</v>
+        <v>-1.660056565915917e-16</v>
       </c>
     </row>
     <row r="12">
@@ -571,7 +571,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C12" t="n">
-        <v>-4.999224230787485e-34</v>
+        <v>-1.84450729546213e-16</v>
       </c>
     </row>
     <row r="13">
@@ -582,7 +582,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>-5.499146653866233e-34</v>
+        <v>-2.028958025008343e-16</v>
       </c>
     </row>
     <row r="14">
@@ -593,7 +593,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C14" t="n">
-        <v>-5.999069076944982e-34</v>
+        <v>-2.213408754554556e-16</v>
       </c>
     </row>
     <row r="15">
@@ -604,7 +604,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C15" t="n">
-        <v>-6.498991500023731e-34</v>
+        <v>-2.397859484100769e-16</v>
       </c>
     </row>
     <row r="16">
@@ -615,7 +615,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C16" t="n">
-        <v>-6.99891392310248e-34</v>
+        <v>-2.582310213646982e-16</v>
       </c>
     </row>
     <row r="17">
@@ -626,7 +626,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C17" t="n">
-        <v>-7.498836346181229e-34</v>
+        <v>-2.766760943193194e-16</v>
       </c>
     </row>
     <row r="18">
@@ -637,7 +637,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C18" t="n">
-        <v>-7.998758769259976e-34</v>
+        <v>-2.951211672739407e-16</v>
       </c>
     </row>
     <row r="19">
@@ -648,7 +648,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C19" t="n">
-        <v>-8.498681192338724e-34</v>
+        <v>-3.13566240228562e-16</v>
       </c>
     </row>
     <row r="20">
@@ -659,7 +659,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C20" t="n">
-        <v>-8.998603615417472e-34</v>
+        <v>-3.320113131831832e-16</v>
       </c>
     </row>
     <row r="21">
@@ -670,7 +670,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C21" t="n">
-        <v>-9.49852603849622e-34</v>
+        <v>-3.504563861378045e-16</v>
       </c>
     </row>
     <row r="22">
@@ -681,7 +681,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C22" t="n">
-        <v>-9.998448461574968e-34</v>
+        <v>-3.689014590924258e-16</v>
       </c>
     </row>
     <row r="23">
@@ -692,7 +692,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.049837088465372e-33</v>
+        <v>-3.87346532047047e-16</v>
       </c>
     </row>
     <row r="24">
@@ -703,7 +703,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.099829330773246e-33</v>
+        <v>-4.057916050016683e-16</v>
       </c>
     </row>
     <row r="25">
@@ -714,7 +714,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C25" t="n">
-        <v>-1.149821573081121e-33</v>
+        <v>-4.242366779562895e-16</v>
       </c>
     </row>
     <row r="26">
@@ -725,7 +725,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.199813815388996e-33</v>
+        <v>-4.426817509109108e-16</v>
       </c>
     </row>
     <row r="27">
@@ -736,7 +736,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C27" t="n">
-        <v>-1.249806057696871e-33</v>
+        <v>-4.611268238655322e-16</v>
       </c>
     </row>
     <row r="28">
@@ -747,7 +747,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.299798300004746e-33</v>
+        <v>-4.795718968201535e-16</v>
       </c>
     </row>
     <row r="29">
@@ -758,7 +758,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.34979054231262e-33</v>
+        <v>-4.980169697747749e-16</v>
       </c>
     </row>
     <row r="30">
@@ -769,7 +769,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.399782784620495e-33</v>
+        <v>-5.164620427293963e-16</v>
       </c>
     </row>
     <row r="31">
@@ -780,7 +780,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.44977502692837e-33</v>
+        <v>-5.349071156840176e-16</v>
       </c>
     </row>
     <row r="32">
@@ -791,7 +791,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.499767269236245e-33</v>
+        <v>-5.53352188638639e-16</v>
       </c>
     </row>
     <row r="33">
@@ -799,10 +799,10 @@
         <v>0.0031</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.54975951154412e-33</v>
+        <v>-5.717972615932603e-16</v>
       </c>
     </row>
     <row r="34">
@@ -810,10 +810,10 @@
         <v>0.0032</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.599751753851994e-33</v>
+        <v>-5.902423345478817e-16</v>
       </c>
     </row>
     <row r="35">
@@ -821,10 +821,10 @@
         <v>0.0033</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.649743996159869e-33</v>
+        <v>-6.086874075025031e-16</v>
       </c>
     </row>
     <row r="36">
@@ -832,10 +832,10 @@
         <v>0.0034</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.699736238467744e-33</v>
+        <v>-6.271324804571243e-16</v>
       </c>
     </row>
     <row r="37">
@@ -843,10 +843,10 @@
         <v>0.0035</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.749728480775619e-33</v>
+        <v>-6.455775534117456e-16</v>
       </c>
     </row>
     <row r="38">
@@ -854,10 +854,10 @@
         <v>0.0036</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C38" t="n">
-        <v>-1.799720723083494e-33</v>
+        <v>-6.640226263663669e-16</v>
       </c>
     </row>
     <row r="39">
@@ -865,10 +865,10 @@
         <v>0.0037</v>
       </c>
       <c r="B39" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C39" t="n">
-        <v>-1.849712965391369e-33</v>
+        <v>-6.824676993209881e-16</v>
       </c>
     </row>
     <row r="40">
@@ -876,10 +876,10 @@
         <v>0.0038</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.899705207699244e-33</v>
+        <v>-7.009127722756094e-16</v>
       </c>
     </row>
     <row r="41">
@@ -887,10 +887,10 @@
         <v>0.0039</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C41" t="n">
-        <v>-1.949697450007119e-33</v>
+        <v>-7.193578452302306e-16</v>
       </c>
     </row>
     <row r="42">
@@ -898,10 +898,10 @@
         <v>0.004</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.999689692314994e-33</v>
+        <v>-7.378029181848519e-16</v>
       </c>
     </row>
     <row r="43">
@@ -909,10 +909,10 @@
         <v>0.0041</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C43" t="n">
-        <v>-2.049681934622869e-33</v>
+        <v>-7.562479911394732e-16</v>
       </c>
     </row>
     <row r="44">
@@ -920,10 +920,10 @@
         <v>0.004200000000000001</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C44" t="n">
-        <v>-2.099674176930744e-33</v>
+        <v>-7.746930640940944e-16</v>
       </c>
     </row>
     <row r="45">
@@ -931,10 +931,10 @@
         <v>0.0043</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C45" t="n">
-        <v>-2.149666419238619e-33</v>
+        <v>-7.931381370487157e-16</v>
       </c>
     </row>
     <row r="46">
@@ -942,10 +942,10 @@
         <v>0.0044</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C46" t="n">
-        <v>-2.199658661546494e-33</v>
+        <v>-8.11583210003337e-16</v>
       </c>
     </row>
     <row r="47">
@@ -953,10 +953,10 @@
         <v>0.004500000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C47" t="n">
-        <v>-2.249650903854369e-33</v>
+        <v>-8.300282829579582e-16</v>
       </c>
     </row>
     <row r="48">
@@ -964,10 +964,10 @@
         <v>0.0046</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C48" t="n">
-        <v>-2.299643146162244e-33</v>
+        <v>-8.484733559125795e-16</v>
       </c>
     </row>
     <row r="49">
@@ -975,10 +975,10 @@
         <v>0.0047</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C49" t="n">
-        <v>-2.349635388470119e-33</v>
+        <v>-8.669184288672007e-16</v>
       </c>
     </row>
     <row r="50">
@@ -986,10 +986,10 @@
         <v>0.0048</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C50" t="n">
-        <v>-2.399627630777994e-33</v>
+        <v>-8.85363501821822e-16</v>
       </c>
     </row>
     <row r="51">
@@ -997,10 +997,10 @@
         <v>0.0049</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C51" t="n">
-        <v>-2.449619873085869e-33</v>
+        <v>-9.038085747764432e-16</v>
       </c>
     </row>
     <row r="52">
@@ -1008,10 +1008,10 @@
         <v>0.005</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C52" t="n">
-        <v>-2.499612115393744e-33</v>
+        <v>-9.222536477310643e-16</v>
       </c>
     </row>
     <row r="53">
@@ -1019,10 +1019,10 @@
         <v>0.0051</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C53" t="n">
-        <v>-2.549604357701619e-33</v>
+        <v>-9.406987206856855e-16</v>
       </c>
     </row>
     <row r="54">
@@ -1030,10 +1030,10 @@
         <v>0.005200000000000001</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999974</v>
       </c>
       <c r="C54" t="n">
-        <v>-2.599596600009494e-33</v>
+        <v>-9.591437936403067e-16</v>
       </c>
     </row>
     <row r="55">
@@ -1041,10 +1041,10 @@
         <v>0.0053</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C55" t="n">
-        <v>-2.649588842317369e-33</v>
+        <v>-9.775888665949278e-16</v>
       </c>
     </row>
     <row r="56">
@@ -1052,10 +1052,10 @@
         <v>0.0054</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999972</v>
       </c>
       <c r="C56" t="n">
-        <v>-2.699581084625244e-33</v>
+        <v>-9.96033939549549e-16</v>
       </c>
     </row>
     <row r="57">
@@ -1063,10 +1063,10 @@
         <v>0.005500000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999971</v>
       </c>
       <c r="C57" t="n">
-        <v>-2.749573326933119e-33</v>
+        <v>-1.01447901250417e-15</v>
       </c>
     </row>
     <row r="58">
@@ -1074,10 +1074,10 @@
         <v>0.0056</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999997</v>
       </c>
       <c r="C58" t="n">
-        <v>-2.799565569240994e-33</v>
+        <v>-1.032924085458791e-15</v>
       </c>
     </row>
     <row r="59">
@@ -1085,10 +1085,10 @@
         <v>0.0057</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999969</v>
       </c>
       <c r="C59" t="n">
-        <v>-2.849557811548869e-33</v>
+        <v>-1.051369158413412e-15</v>
       </c>
     </row>
     <row r="60">
@@ -1096,10 +1096,10 @@
         <v>0.0058</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999968</v>
       </c>
       <c r="C60" t="n">
-        <v>-2.899550053856744e-33</v>
+        <v>-1.069814231368034e-15</v>
       </c>
     </row>
     <row r="61">
@@ -1107,10 +1107,10 @@
         <v>0.0059</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C61" t="n">
-        <v>-2.949542296164619e-33</v>
+        <v>-1.088259304322655e-15</v>
       </c>
     </row>
     <row r="62">
@@ -1118,10 +1118,10 @@
         <v>0.006</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999966</v>
       </c>
       <c r="C62" t="n">
-        <v>-2.999534538472494e-33</v>
+        <v>-1.106704377277276e-15</v>
       </c>
     </row>
     <row r="63">
@@ -1129,10 +1129,10 @@
         <v>0.0061</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C63" t="n">
-        <v>-3.049526780780368e-33</v>
+        <v>-1.125149450231897e-15</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1190,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C3" t="n">
-        <v>-2.434012208463414e-35</v>
+        <v>-8.980499910578066e-18</v>
       </c>
     </row>
     <row r="4">
@@ -1201,7 +1201,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.868024416926842e-35</v>
+        <v>-1.796099982115613e-17</v>
       </c>
     </row>
     <row r="5">
@@ -1212,7 +1212,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.302036625390269e-35</v>
+        <v>-2.69414997317342e-17</v>
       </c>
     </row>
     <row r="6">
@@ -1223,7 +1223,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C6" t="n">
-        <v>-9.736048833853689e-35</v>
+        <v>-3.592199964231226e-17</v>
       </c>
     </row>
     <row r="7">
@@ -1234,7 +1234,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.21700610423171e-34</v>
+        <v>-4.490249955289032e-17</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.460407325078052e-34</v>
+        <v>-5.38829994634684e-17</v>
       </c>
     </row>
     <row r="9">
@@ -1256,7 +1256,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.703808545924393e-34</v>
+        <v>-6.286349937404646e-17</v>
       </c>
     </row>
     <row r="10">
@@ -1267,7 +1267,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.947209766770733e-34</v>
+        <v>-7.18439992846245e-17</v>
       </c>
     </row>
     <row r="11">
@@ -1278,7 +1278,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.190610987617074e-34</v>
+        <v>-8.082449919520258e-17</v>
       </c>
     </row>
     <row r="12">
@@ -1289,7 +1289,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.434012208463414e-34</v>
+        <v>-8.980499910578063e-17</v>
       </c>
     </row>
     <row r="13">
@@ -1300,7 +1300,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.677413429309755e-34</v>
+        <v>-9.878549901635868e-17</v>
       </c>
     </row>
     <row r="14">
@@ -1311,7 +1311,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C14" t="n">
-        <v>-2.920814650156097e-34</v>
+        <v>-1.077659989269367e-16</v>
       </c>
     </row>
     <row r="15">
@@ -1322,7 +1322,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C15" t="n">
-        <v>-3.164215871002439e-34</v>
+        <v>-1.167464988375148e-16</v>
       </c>
     </row>
     <row r="16">
@@ -1333,7 +1333,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C16" t="n">
-        <v>-3.407617091848781e-34</v>
+        <v>-1.257269987480929e-16</v>
       </c>
     </row>
     <row r="17">
@@ -1344,7 +1344,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C17" t="n">
-        <v>-3.651018312695125e-34</v>
+        <v>-1.347074986586709e-16</v>
       </c>
     </row>
     <row r="18">
@@ -1352,10 +1352,10 @@
         <v>0.0007790437238289999</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C18" t="n">
-        <v>-3.894419533541467e-34</v>
+        <v>-1.43687998569249e-16</v>
       </c>
     </row>
     <row r="19">
@@ -1363,10 +1363,10 @@
         <v>0.0008277339565683124</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C19" t="n">
-        <v>-4.137820754387811e-34</v>
+        <v>-1.52668498479827e-16</v>
       </c>
     </row>
     <row r="20">
@@ -1374,10 +1374,10 @@
         <v>0.0008764241893076249</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.381221975234155e-34</v>
+        <v>-1.616489983904051e-16</v>
       </c>
     </row>
     <row r="21">
@@ -1385,10 +1385,10 @@
         <v>0.0009251144220469374</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.6246231960805e-34</v>
+        <v>-1.706294983009831e-16</v>
       </c>
     </row>
     <row r="22">
@@ -1396,10 +1396,10 @@
         <v>0.0009738046547862498</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C22" t="n">
-        <v>-4.868024416926844e-34</v>
+        <v>-1.796099982115611e-16</v>
       </c>
     </row>
     <row r="23">
@@ -1407,10 +1407,10 @@
         <v>0.001022494887525562</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C23" t="n">
-        <v>-5.111425637773186e-34</v>
+        <v>-1.885904981221391e-16</v>
       </c>
     </row>
     <row r="24">
@@ -1418,10 +1418,10 @@
         <v>0.001071185120264875</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C24" t="n">
-        <v>-5.354826858619532e-34</v>
+        <v>-1.975709980327172e-16</v>
       </c>
     </row>
     <row r="25">
@@ -1429,10 +1429,10 @@
         <v>0.001119875353004187</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C25" t="n">
-        <v>-5.598228079465872e-34</v>
+        <v>-2.065514979432952e-16</v>
       </c>
     </row>
     <row r="26">
@@ -1440,10 +1440,10 @@
         <v>0.0011685655857435</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C26" t="n">
-        <v>-5.841629300312216e-34</v>
+        <v>-2.155319978538733e-16</v>
       </c>
     </row>
     <row r="27">
@@ -1451,10 +1451,10 @@
         <v>0.001217255818482812</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C27" t="n">
-        <v>-6.085030521158555e-34</v>
+        <v>-2.245124977644512e-16</v>
       </c>
     </row>
     <row r="28">
@@ -1462,10 +1462,10 @@
         <v>0.001265946051222125</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C28" t="n">
-        <v>-6.3284317420049e-34</v>
+        <v>-2.334929976750294e-16</v>
       </c>
     </row>
     <row r="29">
@@ -1473,10 +1473,10 @@
         <v>0.001314636283961437</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C29" t="n">
-        <v>-6.571832962851239e-34</v>
+        <v>-2.424734975856073e-16</v>
       </c>
     </row>
     <row r="30">
@@ -1484,10 +1484,10 @@
         <v>0.00136332651670075</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C30" t="n">
-        <v>-6.815234183697585e-34</v>
+        <v>-2.514539974961855e-16</v>
       </c>
     </row>
     <row r="31">
@@ -1495,10 +1495,10 @@
         <v>0.001412016749440062</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C31" t="n">
-        <v>-7.058635404543924e-34</v>
+        <v>-2.604344974067633e-16</v>
       </c>
     </row>
     <row r="32">
@@ -1506,10 +1506,10 @@
         <v>0.001460706982179375</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C32" t="n">
-        <v>-7.302036625390268e-34</v>
+        <v>-2.694149973173415e-16</v>
       </c>
     </row>
     <row r="33">
@@ -1517,10 +1517,10 @@
         <v>0.001509397214918687</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C33" t="n">
-        <v>-7.545437846236607e-34</v>
+        <v>-2.783954972279194e-16</v>
       </c>
     </row>
     <row r="34">
@@ -1528,10 +1528,10 @@
         <v>0.001558087447658</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C34" t="n">
-        <v>-7.788839067082951e-34</v>
+        <v>-2.873759971384975e-16</v>
       </c>
     </row>
     <row r="35">
@@ -1539,10 +1539,10 @@
         <v>0.001606777680397312</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C35" t="n">
-        <v>-8.03224028792929e-34</v>
+        <v>-2.963564970490755e-16</v>
       </c>
     </row>
     <row r="36">
@@ -1550,10 +1550,10 @@
         <v>0.001655467913136625</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C36" t="n">
-        <v>-8.275641508775635e-34</v>
+        <v>-3.053369969596536e-16</v>
       </c>
     </row>
     <row r="37">
@@ -1561,10 +1561,10 @@
         <v>0.001704158145875937</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C37" t="n">
-        <v>-8.519042729621974e-34</v>
+        <v>-3.143174968702315e-16</v>
       </c>
     </row>
     <row r="38">
@@ -1572,10 +1572,10 @@
         <v>0.00175284837861525</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C38" t="n">
-        <v>-8.762443950468317e-34</v>
+        <v>-3.232979967808096e-16</v>
       </c>
     </row>
     <row r="39">
@@ -1583,10 +1583,10 @@
         <v>0.001801538611354562</v>
       </c>
       <c r="B39" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C39" t="n">
-        <v>-9.005845171314656e-34</v>
+        <v>-3.322784966913875e-16</v>
       </c>
     </row>
     <row r="40">
@@ -1594,10 +1594,10 @@
         <v>0.001850228844093875</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C40" t="n">
-        <v>-9.249246392161001e-34</v>
+        <v>-3.412589966019657e-16</v>
       </c>
     </row>
     <row r="41">
@@ -1605,10 +1605,10 @@
         <v>0.001898919076833187</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C41" t="n">
-        <v>-9.492647613007338e-34</v>
+        <v>-3.502394965125435e-16</v>
       </c>
     </row>
     <row r="42">
@@ -1616,10 +1616,10 @@
         <v>0.0019476093095725</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C42" t="n">
-        <v>-9.736048833853683e-34</v>
+        <v>-3.592199964231216e-16</v>
       </c>
     </row>
     <row r="43">
@@ -1627,10 +1627,10 @@
         <v>0.001996299542311812</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C43" t="n">
-        <v>-9.979450054700021e-34</v>
+        <v>-3.682004963336996e-16</v>
       </c>
     </row>
     <row r="44">
@@ -1638,10 +1638,10 @@
         <v>0.002044989775051125</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.022285127554636e-33</v>
+        <v>-3.771809962442777e-16</v>
       </c>
     </row>
     <row r="45">
@@ -1649,10 +1649,10 @@
         <v>0.002093680007790437</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.04662524963927e-33</v>
+        <v>-3.861614961548555e-16</v>
       </c>
     </row>
     <row r="46">
@@ -1660,10 +1660,10 @@
         <v>0.00214237024052975</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.070965371723904e-33</v>
+        <v>-3.951419960654337e-16</v>
       </c>
     </row>
     <row r="47">
@@ -1671,10 +1671,10 @@
         <v>0.002191060473269062</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C47" t="n">
-        <v>-1.095305493808538e-33</v>
+        <v>-4.041224959760116e-16</v>
       </c>
     </row>
     <row r="48">
@@ -1682,10 +1682,10 @@
         <v>0.002239750706008375</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.119645615893173e-33</v>
+        <v>-4.131029958865897e-16</v>
       </c>
     </row>
     <row r="49">
@@ -1693,10 +1693,10 @@
         <v>0.002288440938747687</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C49" t="n">
-        <v>-1.143985737977807e-33</v>
+        <v>-4.220834957971676e-16</v>
       </c>
     </row>
     <row r="50">
@@ -1704,10 +1704,10 @@
         <v>0.002337131171487</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C50" t="n">
-        <v>-1.168325860062441e-33</v>
+        <v>-4.310639957077457e-16</v>
       </c>
     </row>
     <row r="51">
@@ -1715,10 +1715,10 @@
         <v>0.002385821404226312</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C51" t="n">
-        <v>-1.192665982147075e-33</v>
+        <v>-4.400444956183236e-16</v>
       </c>
     </row>
     <row r="52">
@@ -1726,10 +1726,10 @@
         <v>0.002434511636965625</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C52" t="n">
-        <v>-1.217006104231709e-33</v>
+        <v>-4.490249955289018e-16</v>
       </c>
     </row>
     <row r="53">
@@ -1737,10 +1737,10 @@
         <v>0.002483201869704937</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C53" t="n">
-        <v>-1.241346226316343e-33</v>
+        <v>-4.580054954394797e-16</v>
       </c>
     </row>
     <row r="54">
@@ -1748,10 +1748,10 @@
         <v>0.00253189210244425</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.265686348400977e-33</v>
+        <v>-4.669859953500579e-16</v>
       </c>
     </row>
     <row r="55">
@@ -1759,10 +1759,10 @@
         <v>0.002580582335183562</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C55" t="n">
-        <v>-1.290026470485611e-33</v>
+        <v>-4.759664952606358e-16</v>
       </c>
     </row>
     <row r="56">
@@ -1770,10 +1770,10 @@
         <v>0.002629272567922875</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C56" t="n">
-        <v>-1.314366592570245e-33</v>
+        <v>-4.849469951712138e-16</v>
       </c>
     </row>
     <row r="57">
@@ -1781,10 +1781,10 @@
         <v>0.002677962800662187</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C57" t="n">
-        <v>-1.338706714654879e-33</v>
+        <v>-4.939274950817917e-16</v>
       </c>
     </row>
     <row r="58">
@@ -1792,10 +1792,10 @@
         <v>0.0027266530334015</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C58" t="n">
-        <v>-1.363046836739514e-33</v>
+        <v>-5.029079949923699e-16</v>
       </c>
     </row>
     <row r="59">
@@ -1803,10 +1803,10 @@
         <v>0.002775343266140812</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C59" t="n">
-        <v>-1.387386958824147e-33</v>
+        <v>-5.118884949029477e-16</v>
       </c>
     </row>
     <row r="60">
@@ -1814,10 +1814,10 @@
         <v>0.002824033498880125</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.411727080908782e-33</v>
+        <v>-5.208689948135257e-16</v>
       </c>
     </row>
     <row r="61">
@@ -1825,10 +1825,10 @@
         <v>0.002872723731619437</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C61" t="n">
-        <v>-1.436067202993415e-33</v>
+        <v>-5.298494947241037e-16</v>
       </c>
     </row>
     <row r="62">
@@ -1836,10 +1836,10 @@
         <v>0.00292141396435875</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C62" t="n">
-        <v>-1.46040732507805e-33</v>
+        <v>-5.388299946346818e-16</v>
       </c>
     </row>
     <row r="63">
@@ -1847,10 +1847,10 @@
         <v>0.002970104197098062</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C63" t="n">
-        <v>-1.484747447162684e-33</v>
+        <v>-5.478104945452597e-16</v>
       </c>
     </row>
     <row r="64">
@@ -1858,10 +1858,10 @@
         <v>0.003018794429837374</v>
       </c>
       <c r="B64" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C64" t="n">
-        <v>-1.509087569247317e-33</v>
+        <v>-5.567909944558377e-16</v>
       </c>
     </row>
     <row r="65">
@@ -1869,10 +1869,10 @@
         <v>0.003067484662576687</v>
       </c>
       <c r="B65" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C65" t="n">
-        <v>-1.533427691331952e-33</v>
+        <v>-5.657714943664158e-16</v>
       </c>
     </row>
     <row r="66">
@@ -1880,10 +1880,10 @@
         <v>0.003116174895315999</v>
       </c>
       <c r="B66" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C66" t="n">
-        <v>-1.557767813416586e-33</v>
+        <v>-5.747519942769937e-16</v>
       </c>
     </row>
     <row r="67">
@@ -1891,10 +1891,10 @@
         <v>0.003164865128055312</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C67" t="n">
-        <v>-1.58210793550122e-33</v>
+        <v>-5.837324941875716e-16</v>
       </c>
     </row>
     <row r="68">
@@ -1902,10 +1902,10 @@
         <v>0.003213555360794625</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C68" t="n">
-        <v>-1.606448057585855e-33</v>
+        <v>-5.927129940981498e-16</v>
       </c>
     </row>
     <row r="69">
@@ -1913,10 +1913,10 @@
         <v>0.003262245593533937</v>
       </c>
       <c r="B69" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C69" t="n">
-        <v>-1.630788179670488e-33</v>
+        <v>-6.016934940087277e-16</v>
       </c>
     </row>
     <row r="70">
@@ -1924,10 +1924,10 @@
         <v>0.00331093582627325</v>
       </c>
       <c r="B70" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C70" t="n">
-        <v>-1.655128301755123e-33</v>
+        <v>-6.106739939193058e-16</v>
       </c>
     </row>
     <row r="71">
@@ -1935,10 +1935,10 @@
         <v>0.003359626059012562</v>
       </c>
       <c r="B71" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C71" t="n">
-        <v>-1.679468423839757e-33</v>
+        <v>-6.196544938298838e-16</v>
       </c>
     </row>
     <row r="72">
@@ -1946,10 +1946,10 @@
         <v>0.003408316291751875</v>
       </c>
       <c r="B72" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C72" t="n">
-        <v>-1.703808545924391e-33</v>
+        <v>-6.286349937404619e-16</v>
       </c>
     </row>
     <row r="73">
@@ -1957,10 +1957,10 @@
         <v>0.003457006524491187</v>
       </c>
       <c r="B73" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C73" t="n">
-        <v>-1.728148668009025e-33</v>
+        <v>-6.376154936510399e-16</v>
       </c>
     </row>
     <row r="74">
@@ -1968,10 +1968,10 @@
         <v>0.0035056967572305</v>
       </c>
       <c r="B74" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C74" t="n">
-        <v>-1.752488790093659e-33</v>
+        <v>-6.465959935616179e-16</v>
       </c>
     </row>
     <row r="75">
@@ -1979,10 +1979,10 @@
         <v>0.003554386989969812</v>
       </c>
       <c r="B75" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C75" t="n">
-        <v>-1.776828912178293e-33</v>
+        <v>-6.555764934721958e-16</v>
       </c>
     </row>
     <row r="76">
@@ -1990,10 +1990,10 @@
         <v>0.003603077222709125</v>
       </c>
       <c r="B76" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C76" t="n">
-        <v>-1.801169034262928e-33</v>
+        <v>-6.64556993382774e-16</v>
       </c>
     </row>
     <row r="77">
@@ -2001,10 +2001,10 @@
         <v>0.003651767455448437</v>
       </c>
       <c r="B77" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C77" t="n">
-        <v>-1.825509156347561e-33</v>
+        <v>-6.735374932933518e-16</v>
       </c>
     </row>
     <row r="78">
@@ -2012,10 +2012,10 @@
         <v>0.00370045768818775</v>
       </c>
       <c r="B78" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C78" t="n">
-        <v>-1.849849278432196e-33</v>
+        <v>-6.8251799320393e-16</v>
       </c>
     </row>
     <row r="79">
@@ -2023,10 +2023,10 @@
         <v>0.003749147920927062</v>
       </c>
       <c r="B79" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C79" t="n">
-        <v>-1.87418940051683e-33</v>
+        <v>-6.914984931145079e-16</v>
       </c>
     </row>
     <row r="80">
@@ -2034,10 +2034,10 @@
         <v>0.003797838153666374</v>
       </c>
       <c r="B80" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C80" t="n">
-        <v>-1.898529522601464e-33</v>
+        <v>-7.004789930250858e-16</v>
       </c>
     </row>
     <row r="81">
@@ -2045,10 +2045,10 @@
         <v>0.003846528386405687</v>
       </c>
       <c r="B81" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C81" t="n">
-        <v>-1.922869644686099e-33</v>
+        <v>-7.09459492935664e-16</v>
       </c>
     </row>
     <row r="82">
@@ -2056,10 +2056,10 @@
         <v>0.003895218619144999</v>
       </c>
       <c r="B82" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C82" t="n">
-        <v>-1.947209766770732e-33</v>
+        <v>-7.184399928462419e-16</v>
       </c>
     </row>
     <row r="83">
@@ -2067,10 +2067,10 @@
         <v>0.003943908851884312</v>
       </c>
       <c r="B83" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C83" t="n">
-        <v>-1.971549888855367e-33</v>
+        <v>-7.274204927568199e-16</v>
       </c>
     </row>
     <row r="84">
@@ -2078,10 +2078,10 @@
         <v>0.003992599084623624</v>
       </c>
       <c r="B84" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C84" t="n">
-        <v>-1.995890010940001e-33</v>
+        <v>-7.364009926673981e-16</v>
       </c>
     </row>
     <row r="85">
@@ -2089,10 +2089,10 @@
         <v>0.004041289317362937</v>
       </c>
       <c r="B85" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C85" t="n">
-        <v>-2.020230133024635e-33</v>
+        <v>-7.453814925779762e-16</v>
       </c>
     </row>
     <row r="86">
@@ -2100,10 +2100,10 @@
         <v>0.00408997955010225</v>
       </c>
       <c r="B86" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C86" t="n">
-        <v>-2.04457025510927e-33</v>
+        <v>-7.543619924885542e-16</v>
       </c>
     </row>
     <row r="87">
@@ -2111,10 +2111,10 @@
         <v>0.004138669782841562</v>
       </c>
       <c r="B87" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C87" t="n">
-        <v>-2.068910377193904e-33</v>
+        <v>-7.63342492399132e-16</v>
       </c>
     </row>
     <row r="88">
@@ -2122,10 +2122,10 @@
         <v>0.004187360015580874</v>
       </c>
       <c r="B88" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C88" t="n">
-        <v>-2.093250499278538e-33</v>
+        <v>-7.723229923097099e-16</v>
       </c>
     </row>
     <row r="89">
@@ -2133,10 +2133,10 @@
         <v>0.004236050248320187</v>
       </c>
       <c r="B89" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C89" t="n">
-        <v>-2.117590621363173e-33</v>
+        <v>-7.813034922202882e-16</v>
       </c>
     </row>
     <row r="90">
@@ -2144,10 +2144,10 @@
         <v>0.004284740481059499</v>
       </c>
       <c r="B90" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C90" t="n">
-        <v>-2.141930743447807e-33</v>
+        <v>-7.902839921308662e-16</v>
       </c>
     </row>
     <row r="91">
@@ -2155,10 +2155,10 @@
         <v>0.004333430713798812</v>
       </c>
       <c r="B91" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C91" t="n">
-        <v>-2.166270865532441e-33</v>
+        <v>-7.992644920414443e-16</v>
       </c>
     </row>
     <row r="92">
@@ -2166,10 +2166,10 @@
         <v>0.004382120946538125</v>
       </c>
       <c r="B92" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C92" t="n">
-        <v>-2.190610987617076e-33</v>
+        <v>-8.082449919520226e-16</v>
       </c>
     </row>
     <row r="93">
@@ -2177,10 +2177,10 @@
         <v>0.004430811179277437</v>
       </c>
       <c r="B93" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C93" t="n">
-        <v>-2.21495110970171e-33</v>
+        <v>-8.172254918626006e-16</v>
       </c>
     </row>
     <row r="94">
@@ -2188,10 +2188,10 @@
         <v>0.004479501412016749</v>
       </c>
       <c r="B94" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C94" t="n">
-        <v>-2.239291231786344e-33</v>
+        <v>-8.262059917731785e-16</v>
       </c>
     </row>
     <row r="95">
@@ -2199,10 +2199,10 @@
         <v>0.004528191644756062</v>
       </c>
       <c r="B95" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C95" t="n">
-        <v>-2.263631353870979e-33</v>
+        <v>-8.351864916837565e-16</v>
       </c>
     </row>
     <row r="96">
@@ -2210,10 +2210,10 @@
         <v>0.004576881877495375</v>
       </c>
       <c r="B96" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C96" t="n">
-        <v>-2.287971475955614e-33</v>
+        <v>-8.441669915943345e-16</v>
       </c>
     </row>
     <row r="97">
@@ -2221,10 +2221,10 @@
         <v>0.004625572110234687</v>
       </c>
       <c r="B97" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C97" t="n">
-        <v>-2.312311598040248e-33</v>
+        <v>-8.531474915049126e-16</v>
       </c>
     </row>
     <row r="98">
@@ -2232,10 +2232,10 @@
         <v>0.004674262342973999</v>
       </c>
       <c r="B98" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C98" t="n">
-        <v>-2.336651720124882e-33</v>
+        <v>-8.621279914154907e-16</v>
       </c>
     </row>
     <row r="99">
@@ -2243,10 +2243,10 @@
         <v>0.004722952575713312</v>
       </c>
       <c r="B99" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C99" t="n">
-        <v>-2.360991842209516e-33</v>
+        <v>-8.711084913260688e-16</v>
       </c>
     </row>
     <row r="100">
@@ -2254,10 +2254,10 @@
         <v>0.004771642808452625</v>
       </c>
       <c r="B100" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C100" t="n">
-        <v>-2.385331964294151e-33</v>
+        <v>-8.800889912366468e-16</v>
       </c>
     </row>
     <row r="101">
@@ -2265,10 +2265,10 @@
         <v>0.004820333041191937</v>
       </c>
       <c r="B101" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C101" t="n">
-        <v>-2.409672086378785e-33</v>
+        <v>-8.890694911472248e-16</v>
       </c>
     </row>
     <row r="102">
@@ -2276,10 +2276,10 @@
         <v>0.004869023273931249</v>
       </c>
       <c r="B102" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C102" t="n">
-        <v>-2.434012208463419e-33</v>
+        <v>-8.980499910578028e-16</v>
       </c>
     </row>
     <row r="103">
@@ -2287,10 +2287,10 @@
         <v>0.004917713506670562</v>
       </c>
       <c r="B103" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C103" t="n">
-        <v>-2.458352330548054e-33</v>
+        <v>-9.07030490968381e-16</v>
       </c>
     </row>
     <row r="104">
@@ -2298,10 +2298,10 @@
         <v>0.004966403739409875</v>
       </c>
       <c r="B104" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C104" t="n">
-        <v>-2.482692452632689e-33</v>
+        <v>-9.160109908789592e-16</v>
       </c>
     </row>
     <row r="105">
@@ -2309,10 +2309,10 @@
         <v>0.005015093972149187</v>
       </c>
       <c r="B105" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999974</v>
       </c>
       <c r="C105" t="n">
-        <v>-2.507032574717322e-33</v>
+        <v>-9.24991490789537e-16</v>
       </c>
     </row>
     <row r="106">
@@ -2320,10 +2320,10 @@
         <v>0.005063784204888499</v>
       </c>
       <c r="B106" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999974</v>
       </c>
       <c r="C106" t="n">
-        <v>-2.531372696801957e-33</v>
+        <v>-9.339719907001151e-16</v>
       </c>
     </row>
     <row r="107">
@@ -2331,10 +2331,10 @@
         <v>0.005112474437627812</v>
       </c>
       <c r="B107" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C107" t="n">
-        <v>-2.555712818886592e-33</v>
+        <v>-9.429524906106933e-16</v>
       </c>
     </row>
     <row r="108">
@@ -2342,10 +2342,10 @@
         <v>0.005161164670367124</v>
       </c>
       <c r="B108" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C108" t="n">
-        <v>-2.580052940971226e-33</v>
+        <v>-9.519329905212713e-16</v>
       </c>
     </row>
     <row r="109">
@@ -2353,10 +2353,10 @@
         <v>0.005209854903106437</v>
       </c>
       <c r="B109" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999972</v>
       </c>
       <c r="C109" t="n">
-        <v>-2.60439306305586e-33</v>
+        <v>-9.609134904318493e-16</v>
       </c>
     </row>
     <row r="110">
@@ -2364,10 +2364,10 @@
         <v>0.005258545135845749</v>
       </c>
       <c r="B110" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999972</v>
       </c>
       <c r="C110" t="n">
-        <v>-2.628733185140495e-33</v>
+        <v>-9.698939903424273e-16</v>
       </c>
     </row>
     <row r="111">
@@ -2375,10 +2375,10 @@
         <v>0.005307235368585062</v>
       </c>
       <c r="B111" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999972</v>
       </c>
       <c r="C111" t="n">
-        <v>-2.653073307225129e-33</v>
+        <v>-9.788744902530055e-16</v>
       </c>
     </row>
     <row r="112">
@@ -2386,10 +2386,10 @@
         <v>0.005355925601324374</v>
       </c>
       <c r="B112" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999971</v>
       </c>
       <c r="C112" t="n">
-        <v>-2.677413429309763e-33</v>
+        <v>-9.878549901635837e-16</v>
       </c>
     </row>
     <row r="113">
@@ -2397,10 +2397,10 @@
         <v>0.005404615834063687</v>
       </c>
       <c r="B113" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999971</v>
       </c>
       <c r="C113" t="n">
-        <v>-2.701753551394398e-33</v>
+        <v>-9.968354900741617e-16</v>
       </c>
     </row>
     <row r="114">
@@ -2408,10 +2408,10 @@
         <v>0.005453306066803</v>
       </c>
       <c r="B114" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999997</v>
       </c>
       <c r="C114" t="n">
-        <v>-2.726093673479033e-33</v>
+        <v>-1.00581598998474e-15</v>
       </c>
     </row>
     <row r="115">
@@ -2419,10 +2419,10 @@
         <v>0.005501996299542311</v>
       </c>
       <c r="B115" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999997</v>
       </c>
       <c r="C115" t="n">
-        <v>-2.750433795563667e-33</v>
+        <v>-1.014796489895318e-15</v>
       </c>
     </row>
     <row r="116">
@@ -2430,10 +2430,10 @@
         <v>0.005550686532281624</v>
       </c>
       <c r="B116" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999969</v>
       </c>
       <c r="C116" t="n">
-        <v>-2.774773917648301e-33</v>
+        <v>-1.023776989805896e-15</v>
       </c>
     </row>
     <row r="117">
@@ -2441,10 +2441,10 @@
         <v>0.005599376765020937</v>
       </c>
       <c r="B117" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999969</v>
       </c>
       <c r="C117" t="n">
-        <v>-2.799114039732936e-33</v>
+        <v>-1.032757489716474e-15</v>
       </c>
     </row>
     <row r="118">
@@ -2452,10 +2452,10 @@
         <v>0.00564806699776025</v>
       </c>
       <c r="B118" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999968</v>
       </c>
       <c r="C118" t="n">
-        <v>-2.82345416181757e-33</v>
+        <v>-1.041737989627052e-15</v>
       </c>
     </row>
     <row r="119">
@@ -2463,10 +2463,10 @@
         <v>0.005696757230499561</v>
       </c>
       <c r="B119" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999968</v>
       </c>
       <c r="C119" t="n">
-        <v>-2.847794283902204e-33</v>
+        <v>-1.05071848953763e-15</v>
       </c>
     </row>
     <row r="120">
@@ -2474,10 +2474,10 @@
         <v>0.005745447463238874</v>
       </c>
       <c r="B120" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C120" t="n">
-        <v>-2.872134405986839e-33</v>
+        <v>-1.059698989448208e-15</v>
       </c>
     </row>
     <row r="121">
@@ -2485,10 +2485,10 @@
         <v>0.005794137695978187</v>
       </c>
       <c r="B121" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C121" t="n">
-        <v>-2.896474528071473e-33</v>
+        <v>-1.068679489358786e-15</v>
       </c>
     </row>
     <row r="122">
@@ -2496,10 +2496,10 @@
         <v>0.0058428279287175</v>
       </c>
       <c r="B122" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999966</v>
       </c>
       <c r="C122" t="n">
-        <v>-2.920814650156108e-33</v>
+        <v>-1.077659989269364e-15</v>
       </c>
     </row>
     <row r="123">
@@ -2507,10 +2507,10 @@
         <v>0.005891518161456812</v>
       </c>
       <c r="B123" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999966</v>
       </c>
       <c r="C123" t="n">
-        <v>-2.945154772240742e-33</v>
+        <v>-1.086640489179942e-15</v>
       </c>
     </row>
     <row r="124">
@@ -2518,10 +2518,10 @@
         <v>0.005940208394196124</v>
       </c>
       <c r="B124" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C124" t="n">
-        <v>-2.969494894325376e-33</v>
+        <v>-1.09562098909052e-15</v>
       </c>
     </row>
     <row r="125">
@@ -2529,10 +2529,10 @@
         <v>0.005988898626935437</v>
       </c>
       <c r="B125" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C125" t="n">
-        <v>-2.993835016410011e-33</v>
+        <v>-1.104601489001098e-15</v>
       </c>
     </row>
     <row r="126">
@@ -2540,10 +2540,10 @@
         <v>0.006037588859674749</v>
       </c>
       <c r="B126" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C126" t="n">
-        <v>-3.018175138494644e-33</v>
+        <v>-1.113581988911676e-15</v>
       </c>
     </row>
     <row r="127">
@@ -2551,10 +2551,10 @@
         <v>0.006086279092414062</v>
       </c>
       <c r="B127" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999964</v>
       </c>
       <c r="C127" t="n">
-        <v>-3.042515260579278e-33</v>
+        <v>-1.122562488822254e-15</v>
       </c>
     </row>
   </sheetData>
@@ -2612,7 +2612,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.998974273742174e-35</v>
+        <v>-1.844415071634524e-17</v>
       </c>
     </row>
     <row r="4">
@@ -2623,7 +2623,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C4" t="n">
-        <v>-9.997948547484348e-35</v>
+        <v>-3.688830143269047e-17</v>
       </c>
     </row>
     <row r="5">
@@ -2634,7 +2634,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.499692282122652e-34</v>
+        <v>-5.53324521490357e-17</v>
       </c>
     </row>
     <row r="6">
@@ -2645,7 +2645,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.99958970949687e-34</v>
+        <v>-7.377660286538093e-17</v>
       </c>
     </row>
     <row r="7">
@@ -2656,7 +2656,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.499487136871087e-34</v>
+        <v>-9.222075358172616e-17</v>
       </c>
     </row>
     <row r="8">
@@ -2667,7 +2667,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.999384564245305e-34</v>
+        <v>-1.106649042980714e-16</v>
       </c>
     </row>
     <row r="9">
@@ -2678,7 +2678,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C9" t="n">
-        <v>-3.499281991619522e-34</v>
+        <v>-1.291090550144166e-16</v>
       </c>
     </row>
     <row r="10">
@@ -2689,7 +2689,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C10" t="n">
-        <v>-3.99917941899374e-34</v>
+        <v>-1.475532057307619e-16</v>
       </c>
     </row>
     <row r="11">
@@ -2700,7 +2700,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.499076846367957e-34</v>
+        <v>-1.659973564471071e-16</v>
       </c>
     </row>
     <row r="12">
@@ -2711,7 +2711,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C12" t="n">
-        <v>-4.998974273742175e-34</v>
+        <v>-1.844415071634523e-16</v>
       </c>
     </row>
     <row r="13">
@@ -2722,7 +2722,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>-5.498871701116392e-34</v>
+        <v>-2.028856578797976e-16</v>
       </c>
     </row>
     <row r="14">
@@ -2733,7 +2733,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C14" t="n">
-        <v>-5.99876912849061e-34</v>
+        <v>-2.213298085961428e-16</v>
       </c>
     </row>
     <row r="15">
@@ -2744,7 +2744,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C15" t="n">
-        <v>-6.498666555864827e-34</v>
+        <v>-2.39773959312488e-16</v>
       </c>
     </row>
     <row r="16">
@@ -2755,7 +2755,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C16" t="n">
-        <v>-6.998563983239045e-34</v>
+        <v>-2.582181100288332e-16</v>
       </c>
     </row>
     <row r="17">
@@ -2766,7 +2766,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C17" t="n">
-        <v>-7.498461410613262e-34</v>
+        <v>-2.766622607451785e-16</v>
       </c>
     </row>
     <row r="18">
@@ -2777,7 +2777,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C18" t="n">
-        <v>-7.99835883798748e-34</v>
+        <v>-2.951064114615237e-16</v>
       </c>
     </row>
     <row r="19">
@@ -2788,7 +2788,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C19" t="n">
-        <v>-8.498256265361697e-34</v>
+        <v>-3.135505621778689e-16</v>
       </c>
     </row>
     <row r="20">
@@ -2799,7 +2799,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C20" t="n">
-        <v>-8.998153692735915e-34</v>
+        <v>-3.319947128942141e-16</v>
       </c>
     </row>
     <row r="21">
@@ -2810,7 +2810,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C21" t="n">
-        <v>-9.498051120110132e-34</v>
+        <v>-3.504388636105593e-16</v>
       </c>
     </row>
     <row r="22">
@@ -2821,7 +2821,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C22" t="n">
-        <v>-9.99794854748435e-34</v>
+        <v>-3.688830143269045e-16</v>
       </c>
     </row>
     <row r="23">
@@ -2832,7 +2832,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.049784597485857e-33</v>
+        <v>-3.873271650432497e-16</v>
       </c>
     </row>
     <row r="24">
@@ -2843,7 +2843,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.099774340223278e-33</v>
+        <v>-4.057713157595949e-16</v>
       </c>
     </row>
     <row r="25">
@@ -2854,7 +2854,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C25" t="n">
-        <v>-1.1497640829607e-33</v>
+        <v>-4.242154664759402e-16</v>
       </c>
     </row>
     <row r="26">
@@ -2865,7 +2865,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.199753825698122e-33</v>
+        <v>-4.426596171922854e-16</v>
       </c>
     </row>
     <row r="27">
@@ -2876,7 +2876,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C27" t="n">
-        <v>-1.249743568435544e-33</v>
+        <v>-4.611037679086306e-16</v>
       </c>
     </row>
     <row r="28">
@@ -2887,7 +2887,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.299733311172965e-33</v>
+        <v>-4.795479186249759e-16</v>
       </c>
     </row>
     <row r="29">
@@ -2898,7 +2898,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.349723053910387e-33</v>
+        <v>-4.979920693413211e-16</v>
       </c>
     </row>
     <row r="30">
@@ -2909,7 +2909,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.399712796647809e-33</v>
+        <v>-5.164362200576664e-16</v>
       </c>
     </row>
     <row r="31">
@@ -2920,7 +2920,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.449702539385231e-33</v>
+        <v>-5.348803707740116e-16</v>
       </c>
     </row>
     <row r="32">
@@ -2928,10 +2928,10 @@
         <v>0.003</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.499692282122652e-33</v>
+        <v>-5.533245214903569e-16</v>
       </c>
     </row>
     <row r="33">
@@ -2939,10 +2939,10 @@
         <v>0.0031</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.549682024860074e-33</v>
+        <v>-5.717686722067022e-16</v>
       </c>
     </row>
     <row r="34">
@@ -2950,10 +2950,10 @@
         <v>0.0032</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.599671767597496e-33</v>
+        <v>-5.902128229230473e-16</v>
       </c>
     </row>
     <row r="35">
@@ -2961,10 +2961,10 @@
         <v>0.0033</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.649661510334918e-33</v>
+        <v>-6.086569736393925e-16</v>
       </c>
     </row>
     <row r="36">
@@ -2972,10 +2972,10 @@
         <v>0.0034</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.699651253072339e-33</v>
+        <v>-6.271011243557377e-16</v>
       </c>
     </row>
     <row r="37">
@@ -2983,10 +2983,10 @@
         <v>0.0035</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.749640995809761e-33</v>
+        <v>-6.455452750720828e-16</v>
       </c>
     </row>
     <row r="38">
@@ -2994,10 +2994,10 @@
         <v>0.0036</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C38" t="n">
-        <v>-1.799630738547183e-33</v>
+        <v>-6.63989425788428e-16</v>
       </c>
     </row>
     <row r="39">
@@ -3005,10 +3005,10 @@
         <v>0.0037</v>
       </c>
       <c r="B39" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C39" t="n">
-        <v>-1.849620481284605e-33</v>
+        <v>-6.824335765047732e-16</v>
       </c>
     </row>
     <row r="40">
@@ -3016,10 +3016,10 @@
         <v>0.0038</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.899610224022026e-33</v>
+        <v>-7.008777272211183e-16</v>
       </c>
     </row>
     <row r="41">
@@ -3027,10 +3027,10 @@
         <v>0.0039</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C41" t="n">
-        <v>-1.949599966759448e-33</v>
+        <v>-7.193218779374635e-16</v>
       </c>
     </row>
     <row r="42">
@@ -3038,10 +3038,10 @@
         <v>0.004</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.99958970949687e-33</v>
+        <v>-7.377660286538086e-16</v>
       </c>
     </row>
     <row r="43">
@@ -3049,10 +3049,10 @@
         <v>0.0041</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C43" t="n">
-        <v>-2.049579452234292e-33</v>
+        <v>-7.562101793701538e-16</v>
       </c>
     </row>
     <row r="44">
@@ -3060,10 +3060,10 @@
         <v>0.004200000000000001</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C44" t="n">
-        <v>-2.099569194971713e-33</v>
+        <v>-7.74654330086499e-16</v>
       </c>
     </row>
     <row r="45">
@@ -3071,10 +3071,10 @@
         <v>0.0043</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C45" t="n">
-        <v>-2.149558937709135e-33</v>
+        <v>-7.930984808028441e-16</v>
       </c>
     </row>
     <row r="46">
@@ -3082,10 +3082,10 @@
         <v>0.0044</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C46" t="n">
-        <v>-2.199548680446557e-33</v>
+        <v>-8.115426315191893e-16</v>
       </c>
     </row>
     <row r="47">
@@ -3093,10 +3093,10 @@
         <v>0.004500000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C47" t="n">
-        <v>-2.249538423183979e-33</v>
+        <v>-8.299867822355345e-16</v>
       </c>
     </row>
     <row r="48">
@@ -3104,10 +3104,10 @@
         <v>0.0046</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C48" t="n">
-        <v>-2.2995281659214e-33</v>
+        <v>-8.484309329518796e-16</v>
       </c>
     </row>
     <row r="49">
@@ -3115,10 +3115,10 @@
         <v>0.0047</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C49" t="n">
-        <v>-2.349517908658822e-33</v>
+        <v>-8.668750836682248e-16</v>
       </c>
     </row>
     <row r="50">
@@ -3126,10 +3126,10 @@
         <v>0.0048</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C50" t="n">
-        <v>-2.399507651396244e-33</v>
+        <v>-8.8531923438457e-16</v>
       </c>
     </row>
     <row r="51">
@@ -3137,10 +3137,10 @@
         <v>0.0049</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C51" t="n">
-        <v>-2.449497394133666e-33</v>
+        <v>-9.037633851009151e-16</v>
       </c>
     </row>
     <row r="52">
@@ -3148,10 +3148,10 @@
         <v>0.005</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C52" t="n">
-        <v>-2.499487136871087e-33</v>
+        <v>-9.222075358172602e-16</v>
       </c>
     </row>
     <row r="53">
@@ -3159,10 +3159,10 @@
         <v>0.0051</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999974</v>
       </c>
       <c r="C53" t="n">
-        <v>-2.549476879608509e-33</v>
+        <v>-9.406516865336053e-16</v>
       </c>
     </row>
     <row r="54">
@@ -3170,10 +3170,10 @@
         <v>0.005200000000000001</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C54" t="n">
-        <v>-2.599466622345931e-33</v>
+        <v>-9.590958372499503e-16</v>
       </c>
     </row>
     <row r="55">
@@ -3181,10 +3181,10 @@
         <v>0.0053</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999972</v>
       </c>
       <c r="C55" t="n">
-        <v>-2.649456365083353e-33</v>
+        <v>-9.775399879662954e-16</v>
       </c>
     </row>
     <row r="56">
@@ -3192,10 +3192,10 @@
         <v>0.0054</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999971</v>
       </c>
       <c r="C56" t="n">
-        <v>-2.699446107820774e-33</v>
+        <v>-9.959841386826405e-16</v>
       </c>
     </row>
     <row r="57">
@@ -3203,10 +3203,10 @@
         <v>0.005500000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999997</v>
       </c>
       <c r="C57" t="n">
-        <v>-2.749435850558196e-33</v>
+        <v>-1.014428289398986e-15</v>
       </c>
     </row>
     <row r="58">
@@ -3214,10 +3214,10 @@
         <v>0.0056</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999969</v>
       </c>
       <c r="C58" t="n">
-        <v>-2.799425593295618e-33</v>
+        <v>-1.032872440115331e-15</v>
       </c>
     </row>
     <row r="59">
@@ -3225,10 +3225,10 @@
         <v>0.0057</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999968</v>
       </c>
       <c r="C59" t="n">
-        <v>-2.84941533603304e-33</v>
+        <v>-1.051316590831676e-15</v>
       </c>
     </row>
     <row r="60">
@@ -3236,10 +3236,10 @@
         <v>0.0058</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C60" t="n">
-        <v>-2.899405078770461e-33</v>
+        <v>-1.069760741548021e-15</v>
       </c>
     </row>
     <row r="61">
@@ -3247,10 +3247,10 @@
         <v>0.0059</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999966</v>
       </c>
       <c r="C61" t="n">
-        <v>-2.949394821507883e-33</v>
+        <v>-1.088204892264366e-15</v>
       </c>
     </row>
     <row r="62">
@@ -3258,10 +3258,10 @@
         <v>0.006</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C62" t="n">
-        <v>-2.999384564245305e-33</v>
+        <v>-1.106649042980711e-15</v>
       </c>
     </row>
     <row r="63">
@@ -3269,10 +3269,10 @@
         <v>0.0061</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999964</v>
       </c>
       <c r="C63" t="n">
-        <v>-3.049374306982727e-33</v>
+        <v>-1.125093193697056e-15</v>
       </c>
     </row>
   </sheetData>
@@ -3331,7 +3331,7 @@
         <v>183</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0003504788812736847</v>
+        <v>0.0003504788812736838</v>
       </c>
       <c r="D2" t="n">
         <v>0.0001</v>
@@ -3349,10 +3349,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0003504788812736847</v>
+        <v>0.0003504788812736834</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -3373,7 +3373,7 @@
         <v>302</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0003504788812736847</v>
+        <v>0.0003504788812736837</v>
       </c>
       <c r="D4" t="n">
         <v>0.0001</v>

</xml_diff>

<commit_message>
Cambios en el ejercicio 1 --- Volumen ya esta resuelto con el diff 3%. Area tiene problemas con un diff de 73,20%
</commit_message>
<xml_diff>
--- a/resultados_tp5_dinamica.xlsx
+++ b/resultados_tp5_dinamica.xlsx
@@ -472,7 +472,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.84450729546213e-17</v>
+        <v>-5.22389559564572e-17</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +483,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.68901459092426e-17</v>
+        <v>-1.044779119129144e-16</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C5" t="n">
-        <v>-5.53352188638639e-17</v>
+        <v>-1.567168678693716e-16</v>
       </c>
     </row>
     <row r="6">
@@ -505,7 +505,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.378029181848519e-17</v>
+        <v>-2.089558238258287e-16</v>
       </c>
     </row>
     <row r="7">
@@ -516,7 +516,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-9.222536477310648e-17</v>
+        <v>-2.611947797822859e-16</v>
       </c>
     </row>
     <row r="8">
@@ -527,7 +527,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.106704377277278e-16</v>
+        <v>-3.134337357387431e-16</v>
       </c>
     </row>
     <row r="9">
@@ -538,7 +538,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.291155106823491e-16</v>
+        <v>-3.656726916952002e-16</v>
       </c>
     </row>
     <row r="10">
@@ -549,7 +549,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.475605836369704e-16</v>
+        <v>-4.179116476516573e-16</v>
       </c>
     </row>
     <row r="11">
@@ -560,7 +560,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.660056565915917e-16</v>
+        <v>-4.701506036081145e-16</v>
       </c>
     </row>
     <row r="12">
@@ -571,7 +571,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.84450729546213e-16</v>
+        <v>-5.223895595645717e-16</v>
       </c>
     </row>
     <row r="13">
@@ -582,7 +582,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.028958025008343e-16</v>
+        <v>-5.746285155210289e-16</v>
       </c>
     </row>
     <row r="14">
@@ -590,10 +590,10 @@
         <v>0.0012</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C14" t="n">
-        <v>-2.213408754554556e-16</v>
+        <v>-6.268674714774861e-16</v>
       </c>
     </row>
     <row r="15">
@@ -601,10 +601,10 @@
         <v>0.0013</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.397859484100769e-16</v>
+        <v>-6.791064274339433e-16</v>
       </c>
     </row>
     <row r="16">
@@ -612,10 +612,10 @@
         <v>0.0014</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.582310213646982e-16</v>
+        <v>-7.313453833904005e-16</v>
       </c>
     </row>
     <row r="17">
@@ -623,10 +623,10 @@
         <v>0.0015</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C17" t="n">
-        <v>-2.766760943193194e-16</v>
+        <v>-7.835843393468577e-16</v>
       </c>
     </row>
     <row r="18">
@@ -634,10 +634,10 @@
         <v>0.0016</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C18" t="n">
-        <v>-2.951211672739407e-16</v>
+        <v>-8.358232953033149e-16</v>
       </c>
     </row>
     <row r="19">
@@ -645,10 +645,10 @@
         <v>0.0017</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C19" t="n">
-        <v>-3.13566240228562e-16</v>
+        <v>-8.88062251259772e-16</v>
       </c>
     </row>
     <row r="20">
@@ -656,10 +656,10 @@
         <v>0.0018</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C20" t="n">
-        <v>-3.320113131831832e-16</v>
+        <v>-9.403012072162291e-16</v>
       </c>
     </row>
     <row r="21">
@@ -667,10 +667,10 @@
         <v>0.0019</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>-3.504563861378045e-16</v>
+        <v>-9.925401631726861e-16</v>
       </c>
     </row>
     <row r="22">
@@ -678,10 +678,10 @@
         <v>0.002</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C22" t="n">
-        <v>-3.689014590924258e-16</v>
+        <v>-1.044779119129143e-15</v>
       </c>
     </row>
     <row r="23">
@@ -689,10 +689,10 @@
         <v>0.0021</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C23" t="n">
-        <v>-3.87346532047047e-16</v>
+        <v>-1.0970180750856e-15</v>
       </c>
     </row>
     <row r="24">
@@ -700,10 +700,10 @@
         <v>0.0022</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C24" t="n">
-        <v>-4.057916050016683e-16</v>
+        <v>-1.149257031042057e-15</v>
       </c>
     </row>
     <row r="25">
@@ -711,10 +711,10 @@
         <v>0.0023</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C25" t="n">
-        <v>-4.242366779562895e-16</v>
+        <v>-1.201495986998514e-15</v>
       </c>
     </row>
     <row r="26">
@@ -722,10 +722,10 @@
         <v>0.0024</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C26" t="n">
-        <v>-4.426817509109108e-16</v>
+        <v>-1.253734942954971e-15</v>
       </c>
     </row>
     <row r="27">
@@ -733,10 +733,10 @@
         <v>0.0025</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C27" t="n">
-        <v>-4.611268238655322e-16</v>
+        <v>-1.305973898911428e-15</v>
       </c>
     </row>
     <row r="28">
@@ -744,10 +744,10 @@
         <v>0.0026</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C28" t="n">
-        <v>-4.795718968201535e-16</v>
+        <v>-1.358212854867885e-15</v>
       </c>
     </row>
     <row r="29">
@@ -755,10 +755,10 @@
         <v>0.0027</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C29" t="n">
-        <v>-4.980169697747749e-16</v>
+        <v>-1.410451810824342e-15</v>
       </c>
     </row>
     <row r="30">
@@ -766,10 +766,10 @@
         <v>0.0028</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C30" t="n">
-        <v>-5.164620427293963e-16</v>
+        <v>-1.462690766780799e-15</v>
       </c>
     </row>
     <row r="31">
@@ -777,10 +777,10 @@
         <v>0.0029</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C31" t="n">
-        <v>-5.349071156840176e-16</v>
+        <v>-1.514929722737256e-15</v>
       </c>
     </row>
     <row r="32">
@@ -788,10 +788,10 @@
         <v>0.003</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C32" t="n">
-        <v>-5.53352188638639e-16</v>
+        <v>-1.567168678693713e-15</v>
       </c>
     </row>
     <row r="33">
@@ -799,10 +799,10 @@
         <v>0.0031</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C33" t="n">
-        <v>-5.717972615932603e-16</v>
+        <v>-1.61940763465017e-15</v>
       </c>
     </row>
     <row r="34">
@@ -810,10 +810,10 @@
         <v>0.0032</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C34" t="n">
-        <v>-5.902423345478817e-16</v>
+        <v>-1.671646590606627e-15</v>
       </c>
     </row>
     <row r="35">
@@ -821,10 +821,10 @@
         <v>0.0033</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C35" t="n">
-        <v>-6.086874075025031e-16</v>
+        <v>-1.723885546563084e-15</v>
       </c>
     </row>
     <row r="36">
@@ -832,10 +832,10 @@
         <v>0.0034</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999971</v>
       </c>
       <c r="C36" t="n">
-        <v>-6.271324804571243e-16</v>
+        <v>-1.776124502519541e-15</v>
       </c>
     </row>
     <row r="37">
@@ -843,10 +843,10 @@
         <v>0.0035</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0.0005257489999999969</v>
       </c>
       <c r="C37" t="n">
-        <v>-6.455775534117456e-16</v>
+        <v>-1.828363458475997e-15</v>
       </c>
     </row>
     <row r="38">
@@ -854,10 +854,10 @@
         <v>0.0036</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C38" t="n">
-        <v>-6.640226263663669e-16</v>
+        <v>-1.880602414432454e-15</v>
       </c>
     </row>
     <row r="39">
@@ -865,10 +865,10 @@
         <v>0.0037</v>
       </c>
       <c r="B39" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C39" t="n">
-        <v>-6.824676993209881e-16</v>
+        <v>-1.932841370388911e-15</v>
       </c>
     </row>
     <row r="40">
@@ -876,10 +876,10 @@
         <v>0.0038</v>
       </c>
       <c r="B40" t="n">
-        <v>0.000525748999999999</v>
+        <v>0.0005257489999999963</v>
       </c>
       <c r="C40" t="n">
-        <v>-7.009127722756094e-16</v>
+        <v>-1.985080326345368e-15</v>
       </c>
     </row>
     <row r="41">
@@ -887,10 +887,10 @@
         <v>0.0039</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0.000525748999999996</v>
       </c>
       <c r="C41" t="n">
-        <v>-7.193578452302306e-16</v>
+        <v>-2.037319282301825e-15</v>
       </c>
     </row>
     <row r="42">
@@ -898,10 +898,10 @@
         <v>0.004</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0.0005257489999999958</v>
       </c>
       <c r="C42" t="n">
-        <v>-7.378029181848519e-16</v>
+        <v>-2.089558238258281e-15</v>
       </c>
     </row>
     <row r="43">
@@ -909,10 +909,10 @@
         <v>0.0041</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0.0005257489999999956</v>
       </c>
       <c r="C43" t="n">
-        <v>-7.562479911394732e-16</v>
+        <v>-2.141797194214738e-15</v>
       </c>
     </row>
     <row r="44">
@@ -920,10 +920,10 @@
         <v>0.004200000000000001</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999985</v>
+        <v>0.0005257489999999954</v>
       </c>
       <c r="C44" t="n">
-        <v>-7.746930640940944e-16</v>
+        <v>-2.194036150171195e-15</v>
       </c>
     </row>
     <row r="45">
@@ -931,10 +931,10 @@
         <v>0.0043</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0.0005257489999999952</v>
       </c>
       <c r="C45" t="n">
-        <v>-7.931381370487157e-16</v>
+        <v>-2.246275106127651e-15</v>
       </c>
     </row>
     <row r="46">
@@ -942,10 +942,10 @@
         <v>0.0044</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0.000525748999999995</v>
       </c>
       <c r="C46" t="n">
-        <v>-8.11583210003337e-16</v>
+        <v>-2.298514062084108e-15</v>
       </c>
     </row>
     <row r="47">
@@ -953,10 +953,10 @@
         <v>0.004500000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0.0005257489999999947</v>
       </c>
       <c r="C47" t="n">
-        <v>-8.300282829579582e-16</v>
+        <v>-2.350753018040564e-15</v>
       </c>
     </row>
     <row r="48">
@@ -964,10 +964,10 @@
         <v>0.0046</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0005257489999999981</v>
+        <v>0.0005257489999999945</v>
       </c>
       <c r="C48" t="n">
-        <v>-8.484733559125795e-16</v>
+        <v>-2.402991973997021e-15</v>
       </c>
     </row>
     <row r="49">
@@ -975,10 +975,10 @@
         <v>0.0047</v>
       </c>
       <c r="B49" t="n">
-        <v>0.000525748999999998</v>
+        <v>0.0005257489999999943</v>
       </c>
       <c r="C49" t="n">
-        <v>-8.669184288672007e-16</v>
+        <v>-2.455230929953477e-15</v>
       </c>
     </row>
     <row r="50">
@@ -986,10 +986,10 @@
         <v>0.0048</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999979</v>
+        <v>0.0005257489999999941</v>
       </c>
       <c r="C50" t="n">
-        <v>-8.85363501821822e-16</v>
+        <v>-2.507469885909933e-15</v>
       </c>
     </row>
     <row r="51">
@@ -997,10 +997,10 @@
         <v>0.0049</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999978</v>
+        <v>0.0005257489999999939</v>
       </c>
       <c r="C51" t="n">
-        <v>-9.038085747764432e-16</v>
+        <v>-2.55970884186639e-15</v>
       </c>
     </row>
     <row r="52">
@@ -1008,10 +1008,10 @@
         <v>0.005</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999977</v>
+        <v>0.0005257489999999937</v>
       </c>
       <c r="C52" t="n">
-        <v>-9.222536477310643e-16</v>
+        <v>-2.611947797822846e-15</v>
       </c>
     </row>
     <row r="53">
@@ -1019,10 +1019,10 @@
         <v>0.0051</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999976</v>
+        <v>0.0005257489999999934</v>
       </c>
       <c r="C53" t="n">
-        <v>-9.406987206856855e-16</v>
+        <v>-2.664186753779303e-15</v>
       </c>
     </row>
     <row r="54">
@@ -1030,10 +1030,10 @@
         <v>0.005200000000000001</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0005257489999999974</v>
+        <v>0.0005257489999999932</v>
       </c>
       <c r="C54" t="n">
-        <v>-9.591437936403067e-16</v>
+        <v>-2.716425709735759e-15</v>
       </c>
     </row>
     <row r="55">
@@ -1041,10 +1041,10 @@
         <v>0.0053</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999973</v>
+        <v>0.0005257489999999929</v>
       </c>
       <c r="C55" t="n">
-        <v>-9.775888665949278e-16</v>
+        <v>-2.768664665692215e-15</v>
       </c>
     </row>
     <row r="56">
@@ -1052,10 +1052,10 @@
         <v>0.0054</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0005257489999999972</v>
+        <v>0.0005257489999999926</v>
       </c>
       <c r="C56" t="n">
-        <v>-9.96033939549549e-16</v>
+        <v>-2.820903621648672e-15</v>
       </c>
     </row>
     <row r="57">
@@ -1063,10 +1063,10 @@
         <v>0.005500000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0005257489999999971</v>
+        <v>0.0005257489999999922</v>
       </c>
       <c r="C57" t="n">
-        <v>-1.01447901250417e-15</v>
+        <v>-2.873142577605128e-15</v>
       </c>
     </row>
     <row r="58">
@@ -1074,10 +1074,10 @@
         <v>0.0056</v>
       </c>
       <c r="B58" t="n">
-        <v>0.000525748999999997</v>
+        <v>0.0005257489999999919</v>
       </c>
       <c r="C58" t="n">
-        <v>-1.032924085458791e-15</v>
+        <v>-2.925381533561584e-15</v>
       </c>
     </row>
     <row r="59">
@@ -1085,10 +1085,10 @@
         <v>0.0057</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999969</v>
+        <v>0.0005257489999999916</v>
       </c>
       <c r="C59" t="n">
-        <v>-1.051369158413412e-15</v>
+        <v>-2.97762048951804e-15</v>
       </c>
     </row>
     <row r="60">
@@ -1096,10 +1096,10 @@
         <v>0.0058</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999968</v>
+        <v>0.0005257489999999913</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.069814231368034e-15</v>
+        <v>-3.029859445474496e-15</v>
       </c>
     </row>
     <row r="61">
@@ -1107,10 +1107,10 @@
         <v>0.0059</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999967</v>
+        <v>0.0005257489999999909</v>
       </c>
       <c r="C61" t="n">
-        <v>-1.088259304322655e-15</v>
+        <v>-3.082098401430952e-15</v>
       </c>
     </row>
     <row r="62">
@@ -1118,10 +1118,10 @@
         <v>0.006</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999966</v>
+        <v>0.0005257489999999906</v>
       </c>
       <c r="C62" t="n">
-        <v>-1.106704377277276e-15</v>
+        <v>-3.134337357387408e-15</v>
       </c>
     </row>
     <row r="63">
@@ -1129,10 +1129,10 @@
         <v>0.0061</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0005257489999999965</v>
+        <v>0.0005257489999999903</v>
       </c>
       <c r="C63" t="n">
-        <v>-1.125149450231897e-15</v>
+        <v>-3.186576313343864e-15</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1190,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C3" t="n">
-        <v>-8.980499910578066e-18</v>
+        <v>-2.543399749352128e-17</v>
       </c>
     </row>
     <row r="4">
@@ -1201,7 +1201,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.796099982115613e-17</v>
+        <v>-5.086799498704255e-17</v>
       </c>
     </row>
     <row r="5">
@@ -1212,7 +1212,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C5" t="n">
-        <v>-2.69414997317342e-17</v>
+        <v>-7.630199248056384e-17</v>
       </c>
     </row>
     <row r="6">
@@ -1223,7 +1223,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.592199964231226e-17</v>
+        <v>-1.017359899740851e-16</v>
       </c>
     </row>
     <row r="7">
@@ -1234,7 +1234,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-4.490249955289032e-17</v>
+        <v>-1.271699874676064e-16</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C8" t="n">
-        <v>-5.38829994634684e-17</v>
+        <v>-1.526039849611276e-16</v>
       </c>
     </row>
     <row r="9">
@@ -1256,7 +1256,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C9" t="n">
-        <v>-6.286349937404646e-17</v>
+        <v>-1.780379824546489e-16</v>
       </c>
     </row>
     <row r="10">
@@ -1267,7 +1267,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C10" t="n">
-        <v>-7.18439992846245e-17</v>
+        <v>-2.034719799481701e-16</v>
       </c>
     </row>
     <row r="11">
@@ -1278,7 +1278,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C11" t="n">
-        <v>-8.082449919520258e-17</v>
+        <v>-2.289059774416914e-16</v>
       </c>
     </row>
     <row r="12">
@@ -1286,10 +1286,10 @@
         <v>0.0004869023273931249</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C12" t="n">
-        <v>-8.980499910578063e-17</v>
+        <v>-2.543399749352126e-16</v>
       </c>
     </row>
     <row r="13">
@@ -1297,10 +1297,10 @@
         <v>0.0005355925601324374</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C13" t="n">
-        <v>-9.878549901635868e-17</v>
+        <v>-2.797739724287338e-16</v>
       </c>
     </row>
     <row r="14">
@@ -1308,10 +1308,10 @@
         <v>0.0005842827928717499</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.077659989269367e-16</v>
+        <v>-3.052079699222551e-16</v>
       </c>
     </row>
     <row r="15">
@@ -1319,10 +1319,10 @@
         <v>0.0006329730256110624</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.167464988375148e-16</v>
+        <v>-3.306419674157764e-16</v>
       </c>
     </row>
     <row r="16">
@@ -1330,10 +1330,10 @@
         <v>0.0006816632583503749</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C16" t="n">
-        <v>-1.257269987480929e-16</v>
+        <v>-3.560759649092976e-16</v>
       </c>
     </row>
     <row r="17">
@@ -1341,10 +1341,10 @@
         <v>0.0007303534910896875</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C17" t="n">
-        <v>-1.347074986586709e-16</v>
+        <v>-3.815099624028188e-16</v>
       </c>
     </row>
     <row r="18">
@@ -1355,7 +1355,7 @@
         <v>0.0005257489999999997</v>
       </c>
       <c r="C18" t="n">
-        <v>-1.43687998569249e-16</v>
+        <v>-4.0694395989634e-16</v>
       </c>
     </row>
     <row r="19">
@@ -1363,10 +1363,10 @@
         <v>0.0008277339565683124</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C19" t="n">
-        <v>-1.52668498479827e-16</v>
+        <v>-4.323779573898612e-16</v>
       </c>
     </row>
     <row r="20">
@@ -1374,10 +1374,10 @@
         <v>0.0008764241893076249</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C20" t="n">
-        <v>-1.616489983904051e-16</v>
+        <v>-4.578119548833825e-16</v>
       </c>
     </row>
     <row r="21">
@@ -1385,10 +1385,10 @@
         <v>0.0009251144220469374</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C21" t="n">
-        <v>-1.706294983009831e-16</v>
+        <v>-4.832459523769035e-16</v>
       </c>
     </row>
     <row r="22">
@@ -1396,10 +1396,10 @@
         <v>0.0009738046547862498</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.796099982115611e-16</v>
+        <v>-5.086799498704248e-16</v>
       </c>
     </row>
     <row r="23">
@@ -1407,10 +1407,10 @@
         <v>0.001022494887525562</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.885904981221391e-16</v>
+        <v>-5.341139473639458e-16</v>
       </c>
     </row>
     <row r="24">
@@ -1418,10 +1418,10 @@
         <v>0.001071185120264875</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.975709980327172e-16</v>
+        <v>-5.595479448574672e-16</v>
       </c>
     </row>
     <row r="25">
@@ -1429,10 +1429,10 @@
         <v>0.001119875353004187</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C25" t="n">
-        <v>-2.065514979432952e-16</v>
+        <v>-5.849819423509883e-16</v>
       </c>
     </row>
     <row r="26">
@@ -1440,10 +1440,10 @@
         <v>0.0011685655857435</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C26" t="n">
-        <v>-2.155319978538733e-16</v>
+        <v>-6.104159398445096e-16</v>
       </c>
     </row>
     <row r="27">
@@ -1451,10 +1451,10 @@
         <v>0.001217255818482812</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C27" t="n">
-        <v>-2.245124977644512e-16</v>
+        <v>-6.358499373380304e-16</v>
       </c>
     </row>
     <row r="28">
@@ -1462,10 +1462,10 @@
         <v>0.001265946051222125</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C28" t="n">
-        <v>-2.334929976750294e-16</v>
+        <v>-6.612839348315519e-16</v>
       </c>
     </row>
     <row r="29">
@@ -1473,10 +1473,10 @@
         <v>0.001314636283961437</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C29" t="n">
-        <v>-2.424734975856073e-16</v>
+        <v>-6.867179323250728e-16</v>
       </c>
     </row>
     <row r="30">
@@ -1484,10 +1484,10 @@
         <v>0.00136332651670075</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C30" t="n">
-        <v>-2.514539974961855e-16</v>
+        <v>-7.121519298185942e-16</v>
       </c>
     </row>
     <row r="31">
@@ -1495,10 +1495,10 @@
         <v>0.001412016749440062</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C31" t="n">
-        <v>-2.604344974067633e-16</v>
+        <v>-7.375859273121151e-16</v>
       </c>
     </row>
     <row r="32">
@@ -1506,10 +1506,10 @@
         <v>0.001460706982179375</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C32" t="n">
-        <v>-2.694149973173415e-16</v>
+        <v>-7.630199248056363e-16</v>
       </c>
     </row>
     <row r="33">
@@ -1517,10 +1517,10 @@
         <v>0.001509397214918687</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C33" t="n">
-        <v>-2.783954972279194e-16</v>
+        <v>-7.884539222991572e-16</v>
       </c>
     </row>
     <row r="34">
@@ -1528,10 +1528,10 @@
         <v>0.001558087447658</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C34" t="n">
-        <v>-2.873759971384975e-16</v>
+        <v>-8.138879197926786e-16</v>
       </c>
     </row>
     <row r="35">
@@ -1539,10 +1539,10 @@
         <v>0.001606777680397312</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C35" t="n">
-        <v>-2.963564970490755e-16</v>
+        <v>-8.393219172861995e-16</v>
       </c>
     </row>
     <row r="36">
@@ -1550,10 +1550,10 @@
         <v>0.001655467913136625</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C36" t="n">
-        <v>-3.053369969596536e-16</v>
+        <v>-8.647559147797208e-16</v>
       </c>
     </row>
     <row r="37">
@@ -1561,10 +1561,10 @@
         <v>0.001704158145875937</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C37" t="n">
-        <v>-3.143174968702315e-16</v>
+        <v>-8.901899122732417e-16</v>
       </c>
     </row>
     <row r="38">
@@ -1572,10 +1572,10 @@
         <v>0.00175284837861525</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C38" t="n">
-        <v>-3.232979967808096e-16</v>
+        <v>-9.156239097667628e-16</v>
       </c>
     </row>
     <row r="39">
@@ -1583,10 +1583,10 @@
         <v>0.001801538611354562</v>
       </c>
       <c r="B39" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C39" t="n">
-        <v>-3.322784966913875e-16</v>
+        <v>-9.410579072602836e-16</v>
       </c>
     </row>
     <row r="40">
@@ -1594,10 +1594,10 @@
         <v>0.001850228844093875</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C40" t="n">
-        <v>-3.412589966019657e-16</v>
+        <v>-9.664919047538051e-16</v>
       </c>
     </row>
     <row r="41">
@@ -1605,10 +1605,10 @@
         <v>0.001898919076833187</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C41" t="n">
-        <v>-3.502394965125435e-16</v>
+        <v>-9.919259022473258e-16</v>
       </c>
     </row>
     <row r="42">
@@ -1616,10 +1616,10 @@
         <v>0.0019476093095725</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C42" t="n">
-        <v>-3.592199964231216e-16</v>
+        <v>-1.017359899740847e-15</v>
       </c>
     </row>
     <row r="43">
@@ -1627,10 +1627,10 @@
         <v>0.001996299542311812</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C43" t="n">
-        <v>-3.682004963336996e-16</v>
+        <v>-1.042793897234368e-15</v>
       </c>
     </row>
     <row r="44">
@@ -1638,10 +1638,10 @@
         <v>0.002044989775051125</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C44" t="n">
-        <v>-3.771809962442777e-16</v>
+        <v>-1.068227894727889e-15</v>
       </c>
     </row>
     <row r="45">
@@ -1649,10 +1649,10 @@
         <v>0.002093680007790437</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C45" t="n">
-        <v>-3.861614961548555e-16</v>
+        <v>-1.09366189222141e-15</v>
       </c>
     </row>
     <row r="46">
@@ -1660,10 +1660,10 @@
         <v>0.00214237024052975</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C46" t="n">
-        <v>-3.951419960654337e-16</v>
+        <v>-1.119095889714931e-15</v>
       </c>
     </row>
     <row r="47">
@@ -1671,10 +1671,10 @@
         <v>0.002191060473269062</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C47" t="n">
-        <v>-4.041224959760116e-16</v>
+        <v>-1.144529887208452e-15</v>
       </c>
     </row>
     <row r="48">
@@ -1682,10 +1682,10 @@
         <v>0.002239750706008375</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C48" t="n">
-        <v>-4.131029958865897e-16</v>
+        <v>-1.169963884701973e-15</v>
       </c>
     </row>
     <row r="49">
@@ -1693,10 +1693,10 @@
         <v>0.002288440938747687</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C49" t="n">
-        <v>-4.220834957971676e-16</v>
+        <v>-1.195397882195494e-15</v>
       </c>
     </row>
     <row r="50">
@@ -1704,10 +1704,10 @@
         <v>0.002337131171487</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C50" t="n">
-        <v>-4.310639957077457e-16</v>
+        <v>-1.220831879689015e-15</v>
       </c>
     </row>
     <row r="51">
@@ -1715,10 +1715,10 @@
         <v>0.002385821404226312</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C51" t="n">
-        <v>-4.400444956183236e-16</v>
+        <v>-1.246265877182536e-15</v>
       </c>
     </row>
     <row r="52">
@@ -1726,10 +1726,10 @@
         <v>0.002434511636965625</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C52" t="n">
-        <v>-4.490249955289018e-16</v>
+        <v>-1.271699874676057e-15</v>
       </c>
     </row>
     <row r="53">
@@ -1737,10 +1737,10 @@
         <v>0.002483201869704937</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C53" t="n">
-        <v>-4.580054954394797e-16</v>
+        <v>-1.297133872169578e-15</v>
       </c>
     </row>
     <row r="54">
@@ -1748,10 +1748,10 @@
         <v>0.00253189210244425</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C54" t="n">
-        <v>-4.669859953500579e-16</v>
+        <v>-1.322567869663099e-15</v>
       </c>
     </row>
     <row r="55">
@@ -1759,10 +1759,10 @@
         <v>0.002580582335183562</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C55" t="n">
-        <v>-4.759664952606358e-16</v>
+        <v>-1.34800186715662e-15</v>
       </c>
     </row>
     <row r="56">
@@ -1770,10 +1770,10 @@
         <v>0.002629272567922875</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C56" t="n">
-        <v>-4.849469951712138e-16</v>
+        <v>-1.373435864650141e-15</v>
       </c>
     </row>
     <row r="57">
@@ -1781,10 +1781,10 @@
         <v>0.002677962800662187</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C57" t="n">
-        <v>-4.939274950817917e-16</v>
+        <v>-1.398869862143662e-15</v>
       </c>
     </row>
     <row r="58">
@@ -1792,10 +1792,10 @@
         <v>0.0027266530334015</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C58" t="n">
-        <v>-5.029079949923699e-16</v>
+        <v>-1.424303859637183e-15</v>
       </c>
     </row>
     <row r="59">
@@ -1803,10 +1803,10 @@
         <v>0.002775343266140812</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C59" t="n">
-        <v>-5.118884949029477e-16</v>
+        <v>-1.449737857130703e-15</v>
       </c>
     </row>
     <row r="60">
@@ -1814,10 +1814,10 @@
         <v>0.002824033498880125</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C60" t="n">
-        <v>-5.208689948135257e-16</v>
+        <v>-1.475171854624224e-15</v>
       </c>
     </row>
     <row r="61">
@@ -1825,10 +1825,10 @@
         <v>0.002872723731619437</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C61" t="n">
-        <v>-5.298494947241037e-16</v>
+        <v>-1.500605852117745e-15</v>
       </c>
     </row>
     <row r="62">
@@ -1836,10 +1836,10 @@
         <v>0.00292141396435875</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C62" t="n">
-        <v>-5.388299946346818e-16</v>
+        <v>-1.526039849611266e-15</v>
       </c>
     </row>
     <row r="63">
@@ -1847,10 +1847,10 @@
         <v>0.002970104197098062</v>
       </c>
       <c r="B63" t="n">
-        <v>0.000525748999999999</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C63" t="n">
-        <v>-5.478104945452597e-16</v>
+        <v>-1.551473847104787e-15</v>
       </c>
     </row>
     <row r="64">
@@ -1858,10 +1858,10 @@
         <v>0.003018794429837374</v>
       </c>
       <c r="B64" t="n">
-        <v>0.000525748999999999</v>
+        <v>0.0005257489999999974</v>
       </c>
       <c r="C64" t="n">
-        <v>-5.567909944558377e-16</v>
+        <v>-1.576907844598308e-15</v>
       </c>
     </row>
     <row r="65">
@@ -1869,10 +1869,10 @@
         <v>0.003067484662576687</v>
       </c>
       <c r="B65" t="n">
-        <v>0.000525748999999999</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C65" t="n">
-        <v>-5.657714943664158e-16</v>
+        <v>-1.602341842091829e-15</v>
       </c>
     </row>
     <row r="66">
@@ -1880,10 +1880,10 @@
         <v>0.003116174895315999</v>
       </c>
       <c r="B66" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C66" t="n">
-        <v>-5.747519942769937e-16</v>
+        <v>-1.627775839585349e-15</v>
       </c>
     </row>
     <row r="67">
@@ -1891,10 +1891,10 @@
         <v>0.003164865128055312</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0.0005257489999999972</v>
       </c>
       <c r="C67" t="n">
-        <v>-5.837324941875716e-16</v>
+        <v>-1.65320983707887e-15</v>
       </c>
     </row>
     <row r="68">
@@ -1902,10 +1902,10 @@
         <v>0.003213555360794625</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0.0005257489999999971</v>
       </c>
       <c r="C68" t="n">
-        <v>-5.927129940981498e-16</v>
+        <v>-1.678643834572392e-15</v>
       </c>
     </row>
     <row r="69">
@@ -1913,10 +1913,10 @@
         <v>0.003262245593533937</v>
       </c>
       <c r="B69" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0.000525748999999997</v>
       </c>
       <c r="C69" t="n">
-        <v>-6.016934940087277e-16</v>
+        <v>-1.704077832065912e-15</v>
       </c>
     </row>
     <row r="70">
@@ -1924,10 +1924,10 @@
         <v>0.00331093582627325</v>
       </c>
       <c r="B70" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0.000525748999999997</v>
       </c>
       <c r="C70" t="n">
-        <v>-6.106739939193058e-16</v>
+        <v>-1.729511829559433e-15</v>
       </c>
     </row>
     <row r="71">
@@ -1935,10 +1935,10 @@
         <v>0.003359626059012562</v>
       </c>
       <c r="B71" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0.0005257489999999969</v>
       </c>
       <c r="C71" t="n">
-        <v>-6.196544938298838e-16</v>
+        <v>-1.754945827052954e-15</v>
       </c>
     </row>
     <row r="72">
@@ -1946,10 +1946,10 @@
         <v>0.003408316291751875</v>
       </c>
       <c r="B72" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0.0005257489999999968</v>
       </c>
       <c r="C72" t="n">
-        <v>-6.286349937404619e-16</v>
+        <v>-1.780379824546475e-15</v>
       </c>
     </row>
     <row r="73">
@@ -1957,10 +1957,10 @@
         <v>0.003457006524491187</v>
       </c>
       <c r="B73" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C73" t="n">
-        <v>-6.376154936510399e-16</v>
+        <v>-1.805813822039996e-15</v>
       </c>
     </row>
     <row r="74">
@@ -1968,10 +1968,10 @@
         <v>0.0035056967572305</v>
       </c>
       <c r="B74" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C74" t="n">
-        <v>-6.465959935616179e-16</v>
+        <v>-1.831247819533517e-15</v>
       </c>
     </row>
     <row r="75">
@@ -1979,10 +1979,10 @@
         <v>0.003554386989969812</v>
       </c>
       <c r="B75" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0.0005257489999999966</v>
       </c>
       <c r="C75" t="n">
-        <v>-6.555764934721958e-16</v>
+        <v>-1.856681817027038e-15</v>
       </c>
     </row>
     <row r="76">
@@ -1990,10 +1990,10 @@
         <v>0.003603077222709125</v>
       </c>
       <c r="B76" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C76" t="n">
-        <v>-6.64556993382774e-16</v>
+        <v>-1.882115814520559e-15</v>
       </c>
     </row>
     <row r="77">
@@ -2001,10 +2001,10 @@
         <v>0.003651767455448437</v>
       </c>
       <c r="B77" t="n">
-        <v>0.0005257489999999985</v>
+        <v>0.0005257489999999964</v>
       </c>
       <c r="C77" t="n">
-        <v>-6.735374932933518e-16</v>
+        <v>-1.907549812014079e-15</v>
       </c>
     </row>
     <row r="78">
@@ -2012,10 +2012,10 @@
         <v>0.00370045768818775</v>
       </c>
       <c r="B78" t="n">
-        <v>0.0005257489999999985</v>
+        <v>0.0005257489999999963</v>
       </c>
       <c r="C78" t="n">
-        <v>-6.8251799320393e-16</v>
+        <v>-1.932983809507601e-15</v>
       </c>
     </row>
     <row r="79">
@@ -2023,10 +2023,10 @@
         <v>0.003749147920927062</v>
       </c>
       <c r="B79" t="n">
-        <v>0.0005257489999999985</v>
+        <v>0.0005257489999999961</v>
       </c>
       <c r="C79" t="n">
-        <v>-6.914984931145079e-16</v>
+        <v>-1.958417807001121e-15</v>
       </c>
     </row>
     <row r="80">
@@ -2034,10 +2034,10 @@
         <v>0.003797838153666374</v>
       </c>
       <c r="B80" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0.000525748999999996</v>
       </c>
       <c r="C80" t="n">
-        <v>-7.004789930250858e-16</v>
+        <v>-1.983851804494642e-15</v>
       </c>
     </row>
     <row r="81">
@@ -2045,10 +2045,10 @@
         <v>0.003846528386405687</v>
       </c>
       <c r="B81" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0.000525748999999996</v>
       </c>
       <c r="C81" t="n">
-        <v>-7.09459492935664e-16</v>
+        <v>-2.009285801988163e-15</v>
       </c>
     </row>
     <row r="82">
@@ -2056,10 +2056,10 @@
         <v>0.003895218619144999</v>
       </c>
       <c r="B82" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0.0005257489999999959</v>
       </c>
       <c r="C82" t="n">
-        <v>-7.184399928462419e-16</v>
+        <v>-2.034719799481684e-15</v>
       </c>
     </row>
     <row r="83">
@@ -2067,10 +2067,10 @@
         <v>0.003943908851884312</v>
       </c>
       <c r="B83" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0.0005257489999999958</v>
       </c>
       <c r="C83" t="n">
-        <v>-7.274204927568199e-16</v>
+        <v>-2.060153796975205e-15</v>
       </c>
     </row>
     <row r="84">
@@ -2078,10 +2078,10 @@
         <v>0.003992599084623624</v>
       </c>
       <c r="B84" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0.0005257489999999957</v>
       </c>
       <c r="C84" t="n">
-        <v>-7.364009926673981e-16</v>
+        <v>-2.085587794468726e-15</v>
       </c>
     </row>
     <row r="85">
@@ -2089,10 +2089,10 @@
         <v>0.004041289317362937</v>
       </c>
       <c r="B85" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0.0005257489999999956</v>
       </c>
       <c r="C85" t="n">
-        <v>-7.453814925779762e-16</v>
+        <v>-2.111021791962247e-15</v>
       </c>
     </row>
     <row r="86">
@@ -2100,10 +2100,10 @@
         <v>0.00408997955010225</v>
       </c>
       <c r="B86" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0.0005257489999999955</v>
       </c>
       <c r="C86" t="n">
-        <v>-7.543619924885542e-16</v>
+        <v>-2.136455789455768e-15</v>
       </c>
     </row>
     <row r="87">
@@ -2111,10 +2111,10 @@
         <v>0.004138669782841562</v>
       </c>
       <c r="B87" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0.0005257489999999954</v>
       </c>
       <c r="C87" t="n">
-        <v>-7.63342492399132e-16</v>
+        <v>-2.161889786949288e-15</v>
       </c>
     </row>
     <row r="88">
@@ -2122,10 +2122,10 @@
         <v>0.004187360015580874</v>
       </c>
       <c r="B88" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0.0005257489999999953</v>
       </c>
       <c r="C88" t="n">
-        <v>-7.723229923097099e-16</v>
+        <v>-2.187323784442809e-15</v>
       </c>
     </row>
     <row r="89">
@@ -2133,10 +2133,10 @@
         <v>0.004236050248320187</v>
       </c>
       <c r="B89" t="n">
-        <v>0.0005257489999999981</v>
+        <v>0.0005257489999999952</v>
       </c>
       <c r="C89" t="n">
-        <v>-7.813034922202882e-16</v>
+        <v>-2.212757781936331e-15</v>
       </c>
     </row>
     <row r="90">
@@ -2144,10 +2144,10 @@
         <v>0.004284740481059499</v>
       </c>
       <c r="B90" t="n">
-        <v>0.0005257489999999981</v>
+        <v>0.0005257489999999951</v>
       </c>
       <c r="C90" t="n">
-        <v>-7.902839921308662e-16</v>
+        <v>-2.238191779429851e-15</v>
       </c>
     </row>
     <row r="91">
@@ -2155,10 +2155,10 @@
         <v>0.004333430713798812</v>
       </c>
       <c r="B91" t="n">
-        <v>0.0005257489999999981</v>
+        <v>0.000525748999999995</v>
       </c>
       <c r="C91" t="n">
-        <v>-7.992644920414443e-16</v>
+        <v>-2.263625776923372e-15</v>
       </c>
     </row>
     <row r="92">
@@ -2166,10 +2166,10 @@
         <v>0.004382120946538125</v>
       </c>
       <c r="B92" t="n">
-        <v>0.000525748999999998</v>
+        <v>0.0005257489999999948</v>
       </c>
       <c r="C92" t="n">
-        <v>-8.082449919520226e-16</v>
+        <v>-2.289059774416894e-15</v>
       </c>
     </row>
     <row r="93">
@@ -2177,10 +2177,10 @@
         <v>0.004430811179277437</v>
       </c>
       <c r="B93" t="n">
-        <v>0.000525748999999998</v>
+        <v>0.0005257489999999947</v>
       </c>
       <c r="C93" t="n">
-        <v>-8.172254918626006e-16</v>
+        <v>-2.314493771910415e-15</v>
       </c>
     </row>
     <row r="94">
@@ -2188,10 +2188,10 @@
         <v>0.004479501412016749</v>
       </c>
       <c r="B94" t="n">
-        <v>0.000525748999999998</v>
+        <v>0.0005257489999999946</v>
       </c>
       <c r="C94" t="n">
-        <v>-8.262059917731785e-16</v>
+        <v>-2.339927769403935e-15</v>
       </c>
     </row>
     <row r="95">
@@ -2199,10 +2199,10 @@
         <v>0.004528191644756062</v>
       </c>
       <c r="B95" t="n">
-        <v>0.0005257489999999979</v>
+        <v>0.0005257489999999945</v>
       </c>
       <c r="C95" t="n">
-        <v>-8.351864916837565e-16</v>
+        <v>-2.365361766897456e-15</v>
       </c>
     </row>
     <row r="96">
@@ -2210,10 +2210,10 @@
         <v>0.004576881877495375</v>
       </c>
       <c r="B96" t="n">
-        <v>0.0005257489999999979</v>
+        <v>0.0005257489999999944</v>
       </c>
       <c r="C96" t="n">
-        <v>-8.441669915943345e-16</v>
+        <v>-2.390795764390977e-15</v>
       </c>
     </row>
     <row r="97">
@@ -2221,10 +2221,10 @@
         <v>0.004625572110234687</v>
       </c>
       <c r="B97" t="n">
-        <v>0.0005257489999999978</v>
+        <v>0.0005257489999999943</v>
       </c>
       <c r="C97" t="n">
-        <v>-8.531474915049126e-16</v>
+        <v>-2.416229761884499e-15</v>
       </c>
     </row>
     <row r="98">
@@ -2232,10 +2232,10 @@
         <v>0.004674262342973999</v>
       </c>
       <c r="B98" t="n">
-        <v>0.0005257489999999978</v>
+        <v>0.0005257489999999942</v>
       </c>
       <c r="C98" t="n">
-        <v>-8.621279914154907e-16</v>
+        <v>-2.441663759378019e-15</v>
       </c>
     </row>
     <row r="99">
@@ -2243,10 +2243,10 @@
         <v>0.004722952575713312</v>
       </c>
       <c r="B99" t="n">
-        <v>0.0005257489999999978</v>
+        <v>0.000525748999999994</v>
       </c>
       <c r="C99" t="n">
-        <v>-8.711084913260688e-16</v>
+        <v>-2.46709775687154e-15</v>
       </c>
     </row>
     <row r="100">
@@ -2254,10 +2254,10 @@
         <v>0.004771642808452625</v>
       </c>
       <c r="B100" t="n">
-        <v>0.0005257489999999977</v>
+        <v>0.0005257489999999939</v>
       </c>
       <c r="C100" t="n">
-        <v>-8.800889912366468e-16</v>
+        <v>-2.492531754365061e-15</v>
       </c>
     </row>
     <row r="101">
@@ -2265,10 +2265,10 @@
         <v>0.004820333041191937</v>
       </c>
       <c r="B101" t="n">
-        <v>0.0005257489999999977</v>
+        <v>0.0005257489999999938</v>
       </c>
       <c r="C101" t="n">
-        <v>-8.890694911472248e-16</v>
+        <v>-2.517965751858582e-15</v>
       </c>
     </row>
     <row r="102">
@@ -2276,10 +2276,10 @@
         <v>0.004869023273931249</v>
       </c>
       <c r="B102" t="n">
-        <v>0.0005257489999999976</v>
+        <v>0.0005257489999999937</v>
       </c>
       <c r="C102" t="n">
-        <v>-8.980499910578028e-16</v>
+        <v>-2.543399749352103e-15</v>
       </c>
     </row>
     <row r="103">
@@ -2287,10 +2287,10 @@
         <v>0.004917713506670562</v>
       </c>
       <c r="B103" t="n">
-        <v>0.0005257489999999976</v>
+        <v>0.0005257489999999935</v>
       </c>
       <c r="C103" t="n">
-        <v>-9.07030490968381e-16</v>
+        <v>-2.568833746845625e-15</v>
       </c>
     </row>
     <row r="104">
@@ -2298,10 +2298,10 @@
         <v>0.004966403739409875</v>
       </c>
       <c r="B104" t="n">
-        <v>0.0005257489999999976</v>
+        <v>0.0005257489999999934</v>
       </c>
       <c r="C104" t="n">
-        <v>-9.160109908789592e-16</v>
+        <v>-2.594267744339145e-15</v>
       </c>
     </row>
     <row r="105">
@@ -2309,10 +2309,10 @@
         <v>0.005015093972149187</v>
       </c>
       <c r="B105" t="n">
-        <v>0.0005257489999999974</v>
+        <v>0.0005257489999999933</v>
       </c>
       <c r="C105" t="n">
-        <v>-9.24991490789537e-16</v>
+        <v>-2.619701741832666e-15</v>
       </c>
     </row>
     <row r="106">
@@ -2320,10 +2320,10 @@
         <v>0.005063784204888499</v>
       </c>
       <c r="B106" t="n">
-        <v>0.0005257489999999974</v>
+        <v>0.0005257489999999931</v>
       </c>
       <c r="C106" t="n">
-        <v>-9.339719907001151e-16</v>
+        <v>-2.645135739326187e-15</v>
       </c>
     </row>
     <row r="107">
@@ -2331,10 +2331,10 @@
         <v>0.005112474437627812</v>
       </c>
       <c r="B107" t="n">
-        <v>0.0005257489999999973</v>
+        <v>0.000525748999999993</v>
       </c>
       <c r="C107" t="n">
-        <v>-9.429524906106933e-16</v>
+        <v>-2.670569736819709e-15</v>
       </c>
     </row>
     <row r="108">
@@ -2342,10 +2342,10 @@
         <v>0.005161164670367124</v>
       </c>
       <c r="B108" t="n">
-        <v>0.0005257489999999973</v>
+        <v>0.0005257489999999929</v>
       </c>
       <c r="C108" t="n">
-        <v>-9.519329905212713e-16</v>
+        <v>-2.696003734313229e-15</v>
       </c>
     </row>
     <row r="109">
@@ -2353,10 +2353,10 @@
         <v>0.005209854903106437</v>
       </c>
       <c r="B109" t="n">
-        <v>0.0005257489999999972</v>
+        <v>0.0005257489999999928</v>
       </c>
       <c r="C109" t="n">
-        <v>-9.609134904318493e-16</v>
+        <v>-2.721437731806751e-15</v>
       </c>
     </row>
     <row r="110">
@@ -2364,10 +2364,10 @@
         <v>0.005258545135845749</v>
       </c>
       <c r="B110" t="n">
-        <v>0.0005257489999999972</v>
+        <v>0.0005257489999999927</v>
       </c>
       <c r="C110" t="n">
-        <v>-9.698939903424273e-16</v>
+        <v>-2.746871729300271e-15</v>
       </c>
     </row>
     <row r="111">
@@ -2375,10 +2375,10 @@
         <v>0.005307235368585062</v>
       </c>
       <c r="B111" t="n">
-        <v>0.0005257489999999972</v>
+        <v>0.0005257489999999925</v>
       </c>
       <c r="C111" t="n">
-        <v>-9.788744902530055e-16</v>
+        <v>-2.772305726793793e-15</v>
       </c>
     </row>
     <row r="112">
@@ -2386,10 +2386,10 @@
         <v>0.005355925601324374</v>
       </c>
       <c r="B112" t="n">
-        <v>0.0005257489999999971</v>
+        <v>0.0005257489999999924</v>
       </c>
       <c r="C112" t="n">
-        <v>-9.878549901635837e-16</v>
+        <v>-2.797739724287314e-15</v>
       </c>
     </row>
     <row r="113">
@@ -2397,10 +2397,10 @@
         <v>0.005404615834063687</v>
       </c>
       <c r="B113" t="n">
-        <v>0.0005257489999999971</v>
+        <v>0.0005257489999999922</v>
       </c>
       <c r="C113" t="n">
-        <v>-9.968354900741617e-16</v>
+        <v>-2.823173721780835e-15</v>
       </c>
     </row>
     <row r="114">
@@ -2408,10 +2408,10 @@
         <v>0.005453306066803</v>
       </c>
       <c r="B114" t="n">
-        <v>0.000525748999999997</v>
+        <v>0.0005257489999999921</v>
       </c>
       <c r="C114" t="n">
-        <v>-1.00581598998474e-15</v>
+        <v>-2.848607719274356e-15</v>
       </c>
     </row>
     <row r="115">
@@ -2419,10 +2419,10 @@
         <v>0.005501996299542311</v>
       </c>
       <c r="B115" t="n">
-        <v>0.000525748999999997</v>
+        <v>0.0005257489999999919</v>
       </c>
       <c r="C115" t="n">
-        <v>-1.014796489895318e-15</v>
+        <v>-2.874041716767876e-15</v>
       </c>
     </row>
     <row r="116">
@@ -2430,10 +2430,10 @@
         <v>0.005550686532281624</v>
       </c>
       <c r="B116" t="n">
-        <v>0.0005257489999999969</v>
+        <v>0.0005257489999999918</v>
       </c>
       <c r="C116" t="n">
-        <v>-1.023776989805896e-15</v>
+        <v>-2.899475714261398e-15</v>
       </c>
     </row>
     <row r="117">
@@ -2441,10 +2441,10 @@
         <v>0.005599376765020937</v>
       </c>
       <c r="B117" t="n">
-        <v>0.0005257489999999969</v>
+        <v>0.0005257489999999917</v>
       </c>
       <c r="C117" t="n">
-        <v>-1.032757489716474e-15</v>
+        <v>-2.924909711754919e-15</v>
       </c>
     </row>
     <row r="118">
@@ -2452,10 +2452,10 @@
         <v>0.00564806699776025</v>
       </c>
       <c r="B118" t="n">
-        <v>0.0005257489999999968</v>
+        <v>0.0005257489999999915</v>
       </c>
       <c r="C118" t="n">
-        <v>-1.041737989627052e-15</v>
+        <v>-2.950343709248439e-15</v>
       </c>
     </row>
     <row r="119">
@@ -2463,10 +2463,10 @@
         <v>0.005696757230499561</v>
       </c>
       <c r="B119" t="n">
-        <v>0.0005257489999999968</v>
+        <v>0.0005257489999999914</v>
       </c>
       <c r="C119" t="n">
-        <v>-1.05071848953763e-15</v>
+        <v>-2.97577770674196e-15</v>
       </c>
     </row>
     <row r="120">
@@ -2474,10 +2474,10 @@
         <v>0.005745447463238874</v>
       </c>
       <c r="B120" t="n">
-        <v>0.0005257489999999967</v>
+        <v>0.0005257489999999913</v>
       </c>
       <c r="C120" t="n">
-        <v>-1.059698989448208e-15</v>
+        <v>-3.001211704235481e-15</v>
       </c>
     </row>
     <row r="121">
@@ -2485,10 +2485,10 @@
         <v>0.005794137695978187</v>
       </c>
       <c r="B121" t="n">
-        <v>0.0005257489999999967</v>
+        <v>0.0005257489999999911</v>
       </c>
       <c r="C121" t="n">
-        <v>-1.068679489358786e-15</v>
+        <v>-3.026645701729002e-15</v>
       </c>
     </row>
     <row r="122">
@@ -2496,10 +2496,10 @@
         <v>0.0058428279287175</v>
       </c>
       <c r="B122" t="n">
-        <v>0.0005257489999999966</v>
+        <v>0.0005257489999999909</v>
       </c>
       <c r="C122" t="n">
-        <v>-1.077659989269364e-15</v>
+        <v>-3.052079699222523e-15</v>
       </c>
     </row>
     <row r="123">
@@ -2507,10 +2507,10 @@
         <v>0.005891518161456812</v>
       </c>
       <c r="B123" t="n">
-        <v>0.0005257489999999966</v>
+        <v>0.0005257489999999908</v>
       </c>
       <c r="C123" t="n">
-        <v>-1.086640489179942e-15</v>
+        <v>-3.077513696716044e-15</v>
       </c>
     </row>
     <row r="124">
@@ -2518,10 +2518,10 @@
         <v>0.005940208394196124</v>
       </c>
       <c r="B124" t="n">
-        <v>0.0005257489999999965</v>
+        <v>0.0005257489999999906</v>
       </c>
       <c r="C124" t="n">
-        <v>-1.09562098909052e-15</v>
+        <v>-3.102947694209565e-15</v>
       </c>
     </row>
     <row r="125">
@@ -2529,10 +2529,10 @@
         <v>0.005988898626935437</v>
       </c>
       <c r="B125" t="n">
-        <v>0.0005257489999999965</v>
+        <v>0.0005257489999999905</v>
       </c>
       <c r="C125" t="n">
-        <v>-1.104601489001098e-15</v>
+        <v>-3.128381691703086e-15</v>
       </c>
     </row>
     <row r="126">
@@ -2540,10 +2540,10 @@
         <v>0.006037588859674749</v>
       </c>
       <c r="B126" t="n">
-        <v>0.0005257489999999965</v>
+        <v>0.0005257489999999903</v>
       </c>
       <c r="C126" t="n">
-        <v>-1.113581988911676e-15</v>
+        <v>-3.153815689196606e-15</v>
       </c>
     </row>
     <row r="127">
@@ -2551,10 +2551,10 @@
         <v>0.006086279092414062</v>
       </c>
       <c r="B127" t="n">
-        <v>0.0005257489999999964</v>
+        <v>0.0005257489999999902</v>
       </c>
       <c r="C127" t="n">
-        <v>-1.122562488822254e-15</v>
+        <v>-3.179249686690127e-15</v>
       </c>
     </row>
   </sheetData>
@@ -2612,7 +2612,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.844415071634524e-17</v>
+        <v>-5.223634405219401e-17</v>
       </c>
     </row>
     <row r="4">
@@ -2623,7 +2623,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C4" t="n">
-        <v>-3.688830143269047e-17</v>
+        <v>-1.04472688104388e-16</v>
       </c>
     </row>
     <row r="5">
@@ -2634,7 +2634,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C5" t="n">
-        <v>-5.53324521490357e-17</v>
+        <v>-1.56709032156582e-16</v>
       </c>
     </row>
     <row r="6">
@@ -2645,7 +2645,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.377660286538093e-17</v>
+        <v>-2.08945376208776e-16</v>
       </c>
     </row>
     <row r="7">
@@ -2656,7 +2656,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C7" t="n">
-        <v>-9.222075358172616e-17</v>
+        <v>-2.6118172026097e-16</v>
       </c>
     </row>
     <row r="8">
@@ -2667,7 +2667,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.106649042980714e-16</v>
+        <v>-3.13418064313164e-16</v>
       </c>
     </row>
     <row r="9">
@@ -2678,7 +2678,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.291090550144166e-16</v>
+        <v>-3.65654408365358e-16</v>
       </c>
     </row>
     <row r="10">
@@ -2689,7 +2689,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.475532057307619e-16</v>
+        <v>-4.17890752417552e-16</v>
       </c>
     </row>
     <row r="11">
@@ -2700,7 +2700,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.659973564471071e-16</v>
+        <v>-4.70127096469746e-16</v>
       </c>
     </row>
     <row r="12">
@@ -2711,7 +2711,7 @@
         <v>0.0005257489999999998</v>
       </c>
       <c r="C12" t="n">
-        <v>-1.844415071634523e-16</v>
+        <v>-5.2236344052194e-16</v>
       </c>
     </row>
     <row r="13">
@@ -2719,10 +2719,10 @@
         <v>0.0011</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999997</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.028856578797976e-16</v>
+        <v>-5.74599784574134e-16</v>
       </c>
     </row>
     <row r="14">
@@ -2730,10 +2730,10 @@
         <v>0.0012</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999996</v>
       </c>
       <c r="C14" t="n">
-        <v>-2.213298085961428e-16</v>
+        <v>-6.26836128626328e-16</v>
       </c>
     </row>
     <row r="15">
@@ -2741,10 +2741,10 @@
         <v>0.0013</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999995</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.39773959312488e-16</v>
+        <v>-6.790724726785219e-16</v>
       </c>
     </row>
     <row r="16">
@@ -2752,10 +2752,10 @@
         <v>0.0014</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999994</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.582181100288332e-16</v>
+        <v>-7.313088167307159e-16</v>
       </c>
     </row>
     <row r="17">
@@ -2763,10 +2763,10 @@
         <v>0.0015</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999993</v>
       </c>
       <c r="C17" t="n">
-        <v>-2.766622607451785e-16</v>
+        <v>-7.835451607829098e-16</v>
       </c>
     </row>
     <row r="18">
@@ -2774,10 +2774,10 @@
         <v>0.0016</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999992</v>
       </c>
       <c r="C18" t="n">
-        <v>-2.951064114615237e-16</v>
+        <v>-8.357815048351037e-16</v>
       </c>
     </row>
     <row r="19">
@@ -2785,10 +2785,10 @@
         <v>0.0017</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999991</v>
       </c>
       <c r="C19" t="n">
-        <v>-3.135505621778689e-16</v>
+        <v>-8.880178488872976e-16</v>
       </c>
     </row>
     <row r="20">
@@ -2796,10 +2796,10 @@
         <v>0.0018</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999999</v>
       </c>
       <c r="C20" t="n">
-        <v>-3.319947128942141e-16</v>
+        <v>-9.402541929394914e-16</v>
       </c>
     </row>
     <row r="21">
@@ -2807,10 +2807,10 @@
         <v>0.0019</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999989</v>
       </c>
       <c r="C21" t="n">
-        <v>-3.504388636105593e-16</v>
+        <v>-9.924905369916852e-16</v>
       </c>
     </row>
     <row r="22">
@@ -2818,10 +2818,10 @@
         <v>0.002</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999988</v>
       </c>
       <c r="C22" t="n">
-        <v>-3.688830143269045e-16</v>
+        <v>-1.044726881043879e-15</v>
       </c>
     </row>
     <row r="23">
@@ -2829,10 +2829,10 @@
         <v>0.0021</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999986</v>
       </c>
       <c r="C23" t="n">
-        <v>-3.873271650432497e-16</v>
+        <v>-1.096963225096073e-15</v>
       </c>
     </row>
     <row r="24">
@@ -2840,10 +2840,10 @@
         <v>0.0022</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999985</v>
       </c>
       <c r="C24" t="n">
-        <v>-4.057713157595949e-16</v>
+        <v>-1.149199569148267e-15</v>
       </c>
     </row>
     <row r="25">
@@ -2851,10 +2851,10 @@
         <v>0.0023</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999984</v>
       </c>
       <c r="C25" t="n">
-        <v>-4.242154664759402e-16</v>
+        <v>-1.20143591320046e-15</v>
       </c>
     </row>
     <row r="26">
@@ -2862,10 +2862,10 @@
         <v>0.0024</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999983</v>
       </c>
       <c r="C26" t="n">
-        <v>-4.426596171922854e-16</v>
+        <v>-1.253672257252654e-15</v>
       </c>
     </row>
     <row r="27">
@@ -2873,10 +2873,10 @@
         <v>0.0025</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999982</v>
       </c>
       <c r="C27" t="n">
-        <v>-4.611037679086306e-16</v>
+        <v>-1.305908601304848e-15</v>
       </c>
     </row>
     <row r="28">
@@ -2884,10 +2884,10 @@
         <v>0.0026</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999981</v>
       </c>
       <c r="C28" t="n">
-        <v>-4.795479186249759e-16</v>
+        <v>-1.358144945357042e-15</v>
       </c>
     </row>
     <row r="29">
@@ -2895,10 +2895,10 @@
         <v>0.0027</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.000525748999999998</v>
       </c>
       <c r="C29" t="n">
-        <v>-4.979920693413211e-16</v>
+        <v>-1.410381289409235e-15</v>
       </c>
     </row>
     <row r="30">
@@ -2906,10 +2906,10 @@
         <v>0.0028</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999979</v>
       </c>
       <c r="C30" t="n">
-        <v>-5.164362200576664e-16</v>
+        <v>-1.462617633461429e-15</v>
       </c>
     </row>
     <row r="31">
@@ -2917,10 +2917,10 @@
         <v>0.0029</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0.0005257489999999978</v>
       </c>
       <c r="C31" t="n">
-        <v>-5.348803707740116e-16</v>
+        <v>-1.514853977513623e-15</v>
       </c>
     </row>
     <row r="32">
@@ -2928,10 +2928,10 @@
         <v>0.003</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0.0005257489999999977</v>
       </c>
       <c r="C32" t="n">
-        <v>-5.533245214903569e-16</v>
+        <v>-1.567090321565817e-15</v>
       </c>
     </row>
     <row r="33">
@@ -2939,10 +2939,10 @@
         <v>0.0031</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0.0005257489999999976</v>
       </c>
       <c r="C33" t="n">
-        <v>-5.717686722067022e-16</v>
+        <v>-1.61932666561801e-15</v>
       </c>
     </row>
     <row r="34">
@@ -2950,10 +2950,10 @@
         <v>0.0032</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0.0005257489999999973</v>
       </c>
       <c r="C34" t="n">
-        <v>-5.902128229230473e-16</v>
+        <v>-1.671563009670204e-15</v>
       </c>
     </row>
     <row r="35">
@@ -2961,10 +2961,10 @@
         <v>0.0033</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0.0005257489999999971</v>
       </c>
       <c r="C35" t="n">
-        <v>-6.086569736393925e-16</v>
+        <v>-1.723799353722398e-15</v>
       </c>
     </row>
     <row r="36">
@@ -2972,10 +2972,10 @@
         <v>0.0034</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0.0005257489999999969</v>
       </c>
       <c r="C36" t="n">
-        <v>-6.271011243557377e-16</v>
+        <v>-1.776035697774591e-15</v>
       </c>
     </row>
     <row r="37">
@@ -2983,10 +2983,10 @@
         <v>0.0035</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0.0005257489999999967</v>
       </c>
       <c r="C37" t="n">
-        <v>-6.455452750720828e-16</v>
+        <v>-1.828272041826785e-15</v>
       </c>
     </row>
     <row r="38">
@@ -2994,10 +2994,10 @@
         <v>0.0036</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0.0005257489999999965</v>
       </c>
       <c r="C38" t="n">
-        <v>-6.63989425788428e-16</v>
+        <v>-1.880508385878978e-15</v>
       </c>
     </row>
     <row r="39">
@@ -3005,10 +3005,10 @@
         <v>0.0037</v>
       </c>
       <c r="B39" t="n">
-        <v>0.000525748999999999</v>
+        <v>0.0005257489999999963</v>
       </c>
       <c r="C39" t="n">
-        <v>-6.824335765047732e-16</v>
+        <v>-1.932744729931172e-15</v>
       </c>
     </row>
     <row r="40">
@@ -3016,10 +3016,10 @@
         <v>0.0038</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0.000525748999999996</v>
       </c>
       <c r="C40" t="n">
-        <v>-7.008777272211183e-16</v>
+        <v>-1.984981073983365e-15</v>
       </c>
     </row>
     <row r="41">
@@ -3027,10 +3027,10 @@
         <v>0.0039</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0.0005257489999999958</v>
       </c>
       <c r="C41" t="n">
-        <v>-7.193218779374635e-16</v>
+        <v>-2.037217418035559e-15</v>
       </c>
     </row>
     <row r="42">
@@ -3038,10 +3038,10 @@
         <v>0.004</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0.0005257489999999956</v>
       </c>
       <c r="C42" t="n">
-        <v>-7.377660286538086e-16</v>
+        <v>-2.089453762087753e-15</v>
       </c>
     </row>
     <row r="43">
@@ -3049,10 +3049,10 @@
         <v>0.0041</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999985</v>
+        <v>0.0005257489999999954</v>
       </c>
       <c r="C43" t="n">
-        <v>-7.562101793701538e-16</v>
+        <v>-2.141690106139946e-15</v>
       </c>
     </row>
     <row r="44">
@@ -3060,10 +3060,10 @@
         <v>0.004200000000000001</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0.0005257489999999952</v>
       </c>
       <c r="C44" t="n">
-        <v>-7.74654330086499e-16</v>
+        <v>-2.193926450192139e-15</v>
       </c>
     </row>
     <row r="45">
@@ -3071,10 +3071,10 @@
         <v>0.0043</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0.000525748999999995</v>
       </c>
       <c r="C45" t="n">
-        <v>-7.930984808028441e-16</v>
+        <v>-2.246162794244332e-15</v>
       </c>
     </row>
     <row r="46">
@@ -3082,10 +3082,10 @@
         <v>0.0044</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0.0005257489999999947</v>
       </c>
       <c r="C46" t="n">
-        <v>-8.115426315191893e-16</v>
+        <v>-2.298399138296526e-15</v>
       </c>
     </row>
     <row r="47">
@@ -3093,10 +3093,10 @@
         <v>0.004500000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999981</v>
+        <v>0.0005257489999999945</v>
       </c>
       <c r="C47" t="n">
-        <v>-8.299867822355345e-16</v>
+        <v>-2.350635482348719e-15</v>
       </c>
     </row>
     <row r="48">
@@ -3104,10 +3104,10 @@
         <v>0.0046</v>
       </c>
       <c r="B48" t="n">
-        <v>0.000525748999999998</v>
+        <v>0.0005257489999999943</v>
       </c>
       <c r="C48" t="n">
-        <v>-8.484309329518796e-16</v>
+        <v>-2.402871826400912e-15</v>
       </c>
     </row>
     <row r="49">
@@ -3115,10 +3115,10 @@
         <v>0.0047</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0005257489999999979</v>
+        <v>0.0005257489999999941</v>
       </c>
       <c r="C49" t="n">
-        <v>-8.668750836682248e-16</v>
+        <v>-2.455108170453105e-15</v>
       </c>
     </row>
     <row r="50">
@@ -3126,10 +3126,10 @@
         <v>0.0048</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999978</v>
+        <v>0.0005257489999999939</v>
       </c>
       <c r="C50" t="n">
-        <v>-8.8531923438457e-16</v>
+        <v>-2.507344514505298e-15</v>
       </c>
     </row>
     <row r="51">
@@ -3137,10 +3137,10 @@
         <v>0.0049</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999977</v>
+        <v>0.0005257489999999937</v>
       </c>
       <c r="C51" t="n">
-        <v>-9.037633851009151e-16</v>
+        <v>-2.559580858557492e-15</v>
       </c>
     </row>
     <row r="52">
@@ -3148,10 +3148,10 @@
         <v>0.005</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999976</v>
+        <v>0.0005257489999999934</v>
       </c>
       <c r="C52" t="n">
-        <v>-9.222075358172602e-16</v>
+        <v>-2.611817202609685e-15</v>
       </c>
     </row>
     <row r="53">
@@ -3159,10 +3159,10 @@
         <v>0.0051</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999974</v>
+        <v>0.0005257489999999932</v>
       </c>
       <c r="C53" t="n">
-        <v>-9.406516865336053e-16</v>
+        <v>-2.664053546661878e-15</v>
       </c>
     </row>
     <row r="54">
@@ -3170,10 +3170,10 @@
         <v>0.005200000000000001</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0005257489999999973</v>
+        <v>0.000525748999999993</v>
       </c>
       <c r="C54" t="n">
-        <v>-9.590958372499503e-16</v>
+        <v>-2.716289890714071e-15</v>
       </c>
     </row>
     <row r="55">
@@ -3181,10 +3181,10 @@
         <v>0.0053</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999972</v>
+        <v>0.0005257489999999927</v>
       </c>
       <c r="C55" t="n">
-        <v>-9.775399879662954e-16</v>
+        <v>-2.768526234766264e-15</v>
       </c>
     </row>
     <row r="56">
@@ -3192,10 +3192,10 @@
         <v>0.0054</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0005257489999999971</v>
+        <v>0.0005257489999999924</v>
       </c>
       <c r="C56" t="n">
-        <v>-9.959841386826405e-16</v>
+        <v>-2.820762578818458e-15</v>
       </c>
     </row>
     <row r="57">
@@ -3203,10 +3203,10 @@
         <v>0.005500000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>0.000525748999999997</v>
+        <v>0.000525748999999992</v>
       </c>
       <c r="C57" t="n">
-        <v>-1.014428289398986e-15</v>
+        <v>-2.87299892287065e-15</v>
       </c>
     </row>
     <row r="58">
@@ -3214,10 +3214,10 @@
         <v>0.0056</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0005257489999999969</v>
+        <v>0.0005257489999999917</v>
       </c>
       <c r="C58" t="n">
-        <v>-1.032872440115331e-15</v>
+        <v>-2.925235266922843e-15</v>
       </c>
     </row>
     <row r="59">
@@ -3225,10 +3225,10 @@
         <v>0.0057</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999968</v>
+        <v>0.0005257489999999914</v>
       </c>
       <c r="C59" t="n">
-        <v>-1.051316590831676e-15</v>
+        <v>-2.977471610975036e-15</v>
       </c>
     </row>
     <row r="60">
@@ -3236,10 +3236,10 @@
         <v>0.0058</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999967</v>
+        <v>0.0005257489999999911</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.069760741548021e-15</v>
+        <v>-3.029707955027229e-15</v>
       </c>
     </row>
     <row r="61">
@@ -3247,10 +3247,10 @@
         <v>0.0059</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999966</v>
+        <v>0.0005257489999999907</v>
       </c>
       <c r="C61" t="n">
-        <v>-1.088204892264366e-15</v>
+        <v>-3.081944299079422e-15</v>
       </c>
     </row>
     <row r="62">
@@ -3258,10 +3258,10 @@
         <v>0.006</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999965</v>
+        <v>0.0005257489999999904</v>
       </c>
       <c r="C62" t="n">
-        <v>-1.106649042980711e-15</v>
+        <v>-3.134180643131614e-15</v>
       </c>
     </row>
     <row r="63">
@@ -3269,10 +3269,10 @@
         <v>0.0061</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0005257489999999964</v>
+        <v>0.0005257489999999901</v>
       </c>
       <c r="C63" t="n">
-        <v>-1.125093193697056e-15</v>
+        <v>-3.186416987183807e-15</v>
       </c>
     </row>
   </sheetData>
@@ -3331,7 +3331,7 @@
         <v>183</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0003504788812736838</v>
+        <v>0.0003504788812736815</v>
       </c>
       <c r="D2" t="n">
         <v>0.0001</v>
@@ -3352,7 +3352,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0003504788812736834</v>
+        <v>0.0003504788812736812</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -3373,7 +3373,7 @@
         <v>302</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0003504788812736837</v>
+        <v>0.0003504788812736814</v>
       </c>
       <c r="D4" t="n">
         <v>0.0001</v>

</xml_diff>

<commit_message>
viendo solucion ejercicio 2
</commit_message>
<xml_diff>
--- a/resultados_tp5_dinamica.xlsx
+++ b/resultados_tp5_dinamica.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -469,670 +469,164 @@
         <v>0.0001</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-5.22389559564572e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.0002</v>
+        <v>0.00022</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.044779119129144e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.0003</v>
+        <v>0.000364</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.567168678693716e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.0004</v>
+        <v>0.0005368</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.089558238258287e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.0005</v>
+        <v>0.00074416</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.611947797822859e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.0006000000000000001</v>
+        <v>0.000992992</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-3.134337357387431e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.0007</v>
+        <v>0.0012915904</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-3.656726916952002e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.0008</v>
+        <v>0.00164990848</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.179116476516573e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.0009000000000000001</v>
+        <v>0.002079890176</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.701506036081145e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.001</v>
+        <v>0.0025958682112</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>-5.223895595645717e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.0011</v>
+        <v>0.00321504185344</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>-5.746285155210289e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.0012</v>
+        <v>0.003958050224128</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>-6.268674714774861e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.0013</v>
+        <v>0.0048496602689536</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>-6.791064274339433e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.0014</v>
+        <v>0.00591959232274432</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>-7.313453833904005e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.0015</v>
+        <v>0.006086279092414062</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>-7.835843393468577e-16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>0.0016</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.0005257489999999993</v>
-      </c>
-      <c r="C18" t="n">
-        <v>-8.358232953033149e-16</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>0.0017</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.0005257489999999992</v>
-      </c>
-      <c r="C19" t="n">
-        <v>-8.88062251259772e-16</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>0.0018</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.0005257489999999991</v>
-      </c>
-      <c r="C20" t="n">
-        <v>-9.403012072162291e-16</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>0.0019</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0.000525748999999999</v>
-      </c>
-      <c r="C21" t="n">
-        <v>-9.925401631726861e-16</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0.0005257489999999989</v>
-      </c>
-      <c r="C22" t="n">
-        <v>-1.044779119129143e-15</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>0.0021</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0.0005257489999999988</v>
-      </c>
-      <c r="C23" t="n">
-        <v>-1.0970180750856e-15</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>0.0022</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0.0005257489999999986</v>
-      </c>
-      <c r="C24" t="n">
-        <v>-1.149257031042057e-15</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>0.0023</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0.0005257489999999985</v>
-      </c>
-      <c r="C25" t="n">
-        <v>-1.201495986998514e-15</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>0.0024</v>
-      </c>
-      <c r="B26" t="n">
-        <v>0.0005257489999999984</v>
-      </c>
-      <c r="C26" t="n">
-        <v>-1.253734942954971e-15</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>0.0025</v>
-      </c>
-      <c r="B27" t="n">
-        <v>0.0005257489999999983</v>
-      </c>
-      <c r="C27" t="n">
-        <v>-1.305973898911428e-15</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>0.0026</v>
-      </c>
-      <c r="B28" t="n">
-        <v>0.0005257489999999982</v>
-      </c>
-      <c r="C28" t="n">
-        <v>-1.358212854867885e-15</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>0.0027</v>
-      </c>
-      <c r="B29" t="n">
-        <v>0.0005257489999999981</v>
-      </c>
-      <c r="C29" t="n">
-        <v>-1.410451810824342e-15</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>0.0028</v>
-      </c>
-      <c r="B30" t="n">
-        <v>0.000525748999999998</v>
-      </c>
-      <c r="C30" t="n">
-        <v>-1.462690766780799e-15</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>0.0029</v>
-      </c>
-      <c r="B31" t="n">
-        <v>0.0005257489999999979</v>
-      </c>
-      <c r="C31" t="n">
-        <v>-1.514929722737256e-15</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="B32" t="n">
-        <v>0.0005257489999999978</v>
-      </c>
-      <c r="C32" t="n">
-        <v>-1.567168678693713e-15</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>0.0031</v>
-      </c>
-      <c r="B33" t="n">
-        <v>0.0005257489999999977</v>
-      </c>
-      <c r="C33" t="n">
-        <v>-1.61940763465017e-15</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>0.0032</v>
-      </c>
-      <c r="B34" t="n">
-        <v>0.0005257489999999976</v>
-      </c>
-      <c r="C34" t="n">
-        <v>-1.671646590606627e-15</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>0.0033</v>
-      </c>
-      <c r="B35" t="n">
-        <v>0.0005257489999999973</v>
-      </c>
-      <c r="C35" t="n">
-        <v>-1.723885546563084e-15</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>0.0034</v>
-      </c>
-      <c r="B36" t="n">
-        <v>0.0005257489999999971</v>
-      </c>
-      <c r="C36" t="n">
-        <v>-1.776124502519541e-15</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>0.0035</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0.0005257489999999969</v>
-      </c>
-      <c r="C37" t="n">
-        <v>-1.828363458475997e-15</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>0.0036</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0.0005257489999999967</v>
-      </c>
-      <c r="C38" t="n">
-        <v>-1.880602414432454e-15</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>0.0037</v>
-      </c>
-      <c r="B39" t="n">
-        <v>0.0005257489999999965</v>
-      </c>
-      <c r="C39" t="n">
-        <v>-1.932841370388911e-15</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>0.0038</v>
-      </c>
-      <c r="B40" t="n">
-        <v>0.0005257489999999963</v>
-      </c>
-      <c r="C40" t="n">
-        <v>-1.985080326345368e-15</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>0.0039</v>
-      </c>
-      <c r="B41" t="n">
-        <v>0.000525748999999996</v>
-      </c>
-      <c r="C41" t="n">
-        <v>-2.037319282301825e-15</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="B42" t="n">
-        <v>0.0005257489999999958</v>
-      </c>
-      <c r="C42" t="n">
-        <v>-2.089558238258281e-15</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>0.0041</v>
-      </c>
-      <c r="B43" t="n">
-        <v>0.0005257489999999956</v>
-      </c>
-      <c r="C43" t="n">
-        <v>-2.141797194214738e-15</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>0.004200000000000001</v>
-      </c>
-      <c r="B44" t="n">
-        <v>0.0005257489999999954</v>
-      </c>
-      <c r="C44" t="n">
-        <v>-2.194036150171195e-15</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>0.0043</v>
-      </c>
-      <c r="B45" t="n">
-        <v>0.0005257489999999952</v>
-      </c>
-      <c r="C45" t="n">
-        <v>-2.246275106127651e-15</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>0.0044</v>
-      </c>
-      <c r="B46" t="n">
-        <v>0.000525748999999995</v>
-      </c>
-      <c r="C46" t="n">
-        <v>-2.298514062084108e-15</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>0.004500000000000001</v>
-      </c>
-      <c r="B47" t="n">
-        <v>0.0005257489999999947</v>
-      </c>
-      <c r="C47" t="n">
-        <v>-2.350753018040564e-15</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>0.0046</v>
-      </c>
-      <c r="B48" t="n">
-        <v>0.0005257489999999945</v>
-      </c>
-      <c r="C48" t="n">
-        <v>-2.402991973997021e-15</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>0.0047</v>
-      </c>
-      <c r="B49" t="n">
-        <v>0.0005257489999999943</v>
-      </c>
-      <c r="C49" t="n">
-        <v>-2.455230929953477e-15</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>0.0048</v>
-      </c>
-      <c r="B50" t="n">
-        <v>0.0005257489999999941</v>
-      </c>
-      <c r="C50" t="n">
-        <v>-2.507469885909933e-15</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>0.0049</v>
-      </c>
-      <c r="B51" t="n">
-        <v>0.0005257489999999939</v>
-      </c>
-      <c r="C51" t="n">
-        <v>-2.55970884186639e-15</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="B52" t="n">
-        <v>0.0005257489999999937</v>
-      </c>
-      <c r="C52" t="n">
-        <v>-2.611947797822846e-15</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>0.0051</v>
-      </c>
-      <c r="B53" t="n">
-        <v>0.0005257489999999934</v>
-      </c>
-      <c r="C53" t="n">
-        <v>-2.664186753779303e-15</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>0.005200000000000001</v>
-      </c>
-      <c r="B54" t="n">
-        <v>0.0005257489999999932</v>
-      </c>
-      <c r="C54" t="n">
-        <v>-2.716425709735759e-15</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>0.0053</v>
-      </c>
-      <c r="B55" t="n">
-        <v>0.0005257489999999929</v>
-      </c>
-      <c r="C55" t="n">
-        <v>-2.768664665692215e-15</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>0.0054</v>
-      </c>
-      <c r="B56" t="n">
-        <v>0.0005257489999999926</v>
-      </c>
-      <c r="C56" t="n">
-        <v>-2.820903621648672e-15</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>0.005500000000000001</v>
-      </c>
-      <c r="B57" t="n">
-        <v>0.0005257489999999922</v>
-      </c>
-      <c r="C57" t="n">
-        <v>-2.873142577605128e-15</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>0.0056</v>
-      </c>
-      <c r="B58" t="n">
-        <v>0.0005257489999999919</v>
-      </c>
-      <c r="C58" t="n">
-        <v>-2.925381533561584e-15</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>0.0057</v>
-      </c>
-      <c r="B59" t="n">
-        <v>0.0005257489999999916</v>
-      </c>
-      <c r="C59" t="n">
-        <v>-2.97762048951804e-15</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>0.0058</v>
-      </c>
-      <c r="B60" t="n">
-        <v>0.0005257489999999913</v>
-      </c>
-      <c r="C60" t="n">
-        <v>-3.029859445474496e-15</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>0.0059</v>
-      </c>
-      <c r="B61" t="n">
-        <v>0.0005257489999999909</v>
-      </c>
-      <c r="C61" t="n">
-        <v>-3.082098401430952e-15</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>0.006</v>
-      </c>
-      <c r="B62" t="n">
-        <v>0.0005257489999999906</v>
-      </c>
-      <c r="C62" t="n">
-        <v>-3.134337357387408e-15</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>0.0061</v>
-      </c>
-      <c r="B63" t="n">
-        <v>0.0005257489999999903</v>
-      </c>
-      <c r="C63" t="n">
-        <v>-3.186576313343864e-15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -1187,10 +681,10 @@
         <v>4.869023273931249e-05</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-2.543399749352128e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1198,10 +692,10 @@
         <v>9.738046547862498e-05</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-5.086799498704255e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1209,10 +703,10 @@
         <v>0.0001460706982179375</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-7.630199248056384e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1220,10 +714,10 @@
         <v>0.00019476093095725</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.017359899740851e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1231,10 +725,10 @@
         <v>0.0002434511636965625</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.271699874676064e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1242,10 +736,10 @@
         <v>0.000292141396435875</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.526039849611277e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1253,10 +747,10 @@
         <v>0.0003408316291751875</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.780379824546489e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1264,10 +758,10 @@
         <v>0.0003895218619144999</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.034719799481701e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1275,10 +769,10 @@
         <v>0.0004382120946538125</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.289059774416914e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1286,10 +780,10 @@
         <v>0.0004869023273931249</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.543399749352127e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1297,10 +791,10 @@
         <v>0.0005355925601324374</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>-2.797739724287339e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1308,10 +802,10 @@
         <v>0.0005842827928717499</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>-3.052079699222551e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1319,10 +813,10 @@
         <v>0.0006329730256110624</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>-3.306419674157764e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1330,10 +824,10 @@
         <v>0.0006816632583503749</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>-3.560759649092976e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1341,10 +835,10 @@
         <v>0.0007303534910896875</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>-3.815099624028189e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1352,10 +846,10 @@
         <v>0.0007790437238289999</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>-4.069439598963401e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1363,10 +857,10 @@
         <v>0.0008277339565683124</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>-4.323779573898614e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1374,10 +868,10 @@
         <v>0.0008764241893076249</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>-4.578119548833826e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1385,10 +879,10 @@
         <v>0.0009251144220469374</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.832459523769037e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1396,10 +890,10 @@
         <v>0.0009738046547862498</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>-5.086799498704249e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1407,10 +901,10 @@
         <v>0.001022494887525562</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>-5.34113947363946e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1418,10 +912,10 @@
         <v>0.001071185120264875</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>-5.595479448574674e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1429,10 +923,10 @@
         <v>0.001119875353004187</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>-5.849819423509884e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1440,10 +934,10 @@
         <v>0.0011685655857435</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>-6.104159398445097e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1451,10 +945,10 @@
         <v>0.001217255818482812</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>-6.358499373380306e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1462,10 +956,10 @@
         <v>0.001265946051222125</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>-6.612839348315521e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1473,10 +967,10 @@
         <v>0.001314636283961437</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>-6.867179323250729e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1484,10 +978,10 @@
         <v>0.00136332651670075</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>-7.121519298185944e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1495,10 +989,10 @@
         <v>0.001412016749440062</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>-7.375859273121153e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1506,10 +1000,10 @@
         <v>0.001460706982179375</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>-7.630199248056366e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1517,10 +1011,10 @@
         <v>0.001509397214918687</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>-7.884539222991574e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1528,10 +1022,10 @@
         <v>0.001558087447658</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>-8.138879197926788e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1539,10 +1033,10 @@
         <v>0.001606777680397312</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>-8.393219172861997e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1550,10 +1044,10 @@
         <v>0.001655467913136625</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>-8.64755914779721e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1561,10 +1055,10 @@
         <v>0.001704158145875937</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>-8.901899122732419e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1572,10 +1066,10 @@
         <v>0.00175284837861525</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>-9.156239097667632e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1583,10 +1077,10 @@
         <v>0.001801538611354562</v>
       </c>
       <c r="B39" t="n">
-        <v>0.000525748999999999</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>-9.41057907260284e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1594,10 +1088,10 @@
         <v>0.001850228844093875</v>
       </c>
       <c r="B40" t="n">
-        <v>0.000525748999999999</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>-9.664919047538055e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1605,10 +1099,10 @@
         <v>0.001898919076833187</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>-9.919259022473262e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1616,10 +1110,10 @@
         <v>0.0019476093095725</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.017359899740847e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1627,10 +1121,10 @@
         <v>0.001996299542311812</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>-1.042793897234368e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1638,10 +1132,10 @@
         <v>0.002044989775051125</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.06822789472789e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1649,10 +1143,10 @@
         <v>0.002093680007790437</v>
       </c>
       <c r="B45" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.09366189222141e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1660,10 +1154,10 @@
         <v>0.00214237024052975</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.119095889714931e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1671,10 +1165,10 @@
         <v>0.002191060473269062</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>-1.144529887208452e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1682,10 +1176,10 @@
         <v>0.002239750706008375</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0005257489999999985</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.169963884701974e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1693,10 +1187,10 @@
         <v>0.002288440938747687</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>-1.195397882195494e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1704,10 +1198,10 @@
         <v>0.002337131171487</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>-1.220831879689015e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1715,10 +1209,10 @@
         <v>0.002385821404226312</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>-1.246265877182536e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1726,10 +1220,10 @@
         <v>0.002434511636965625</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>-1.271699874676057e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1737,10 +1231,10 @@
         <v>0.002483201869704937</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>-1.297133872169578e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1748,10 +1242,10 @@
         <v>0.00253189210244425</v>
       </c>
       <c r="B54" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.322567869663099e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1759,10 +1253,10 @@
         <v>0.002580582335183562</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999981</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>-1.34800186715662e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1770,10 +1264,10 @@
         <v>0.002629272567922875</v>
       </c>
       <c r="B56" t="n">
-        <v>0.000525748999999998</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>-1.373435864650141e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1781,10 +1275,10 @@
         <v>0.002677962800662187</v>
       </c>
       <c r="B57" t="n">
-        <v>0.000525748999999998</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>-1.398869862143662e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1792,10 +1286,10 @@
         <v>0.0027266530334015</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0005257489999999979</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>-1.424303859637183e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1803,10 +1297,10 @@
         <v>0.002775343266140812</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999979</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>-1.449737857130704e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1814,10 +1308,10 @@
         <v>0.002824033498880125</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999978</v>
+        <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>-1.475171854624224e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1825,10 +1319,10 @@
         <v>0.002872723731619437</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999977</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>-1.500605852117745e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1836,10 +1330,10 @@
         <v>0.00292141396435875</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999977</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>-1.526039849611266e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1847,10 +1341,10 @@
         <v>0.002970104197098062</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0005257489999999976</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>-1.551473847104787e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1858,10 +1352,10 @@
         <v>0.003018794429837374</v>
       </c>
       <c r="B64" t="n">
-        <v>0.0005257489999999974</v>
+        <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>-1.576907844598308e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1869,10 +1363,10 @@
         <v>0.003067484662576687</v>
       </c>
       <c r="B65" t="n">
-        <v>0.0005257489999999973</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>-1.602341842091829e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1880,10 +1374,10 @@
         <v>0.003116174895315999</v>
       </c>
       <c r="B66" t="n">
-        <v>0.0005257489999999973</v>
+        <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>-1.627775839585349e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1891,10 +1385,10 @@
         <v>0.003164865128055312</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0005257489999999972</v>
+        <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>-1.65320983707887e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1902,10 +1396,10 @@
         <v>0.003213555360794625</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0005257489999999971</v>
+        <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>-1.678643834572391e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1913,10 +1407,10 @@
         <v>0.003262245593533937</v>
       </c>
       <c r="B69" t="n">
-        <v>0.000525748999999997</v>
+        <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>-1.704077832065912e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1924,10 +1418,10 @@
         <v>0.00331093582627325</v>
       </c>
       <c r="B70" t="n">
-        <v>0.000525748999999997</v>
+        <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>-1.729511829559433e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1935,10 +1429,10 @@
         <v>0.003359626059012562</v>
       </c>
       <c r="B71" t="n">
-        <v>0.0005257489999999969</v>
+        <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>-1.754945827052954e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1946,10 +1440,10 @@
         <v>0.003408316291751875</v>
       </c>
       <c r="B72" t="n">
-        <v>0.0005257489999999968</v>
+        <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>-1.780379824546475e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1957,10 +1451,10 @@
         <v>0.003457006524491187</v>
       </c>
       <c r="B73" t="n">
-        <v>0.0005257489999999967</v>
+        <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>-1.805813822039995e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1968,10 +1462,10 @@
         <v>0.0035056967572305</v>
       </c>
       <c r="B74" t="n">
-        <v>0.0005257489999999967</v>
+        <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>-1.831247819533516e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1979,10 +1473,10 @@
         <v>0.003554386989969812</v>
       </c>
       <c r="B75" t="n">
-        <v>0.0005257489999999966</v>
+        <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>-1.856681817027037e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1990,10 +1484,10 @@
         <v>0.003603077222709125</v>
       </c>
       <c r="B76" t="n">
-        <v>0.0005257489999999965</v>
+        <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>-1.882115814520558e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2001,10 +1495,10 @@
         <v>0.003651767455448437</v>
       </c>
       <c r="B77" t="n">
-        <v>0.0005257489999999964</v>
+        <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>-1.907549812014079e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2012,10 +1506,10 @@
         <v>0.00370045768818775</v>
       </c>
       <c r="B78" t="n">
-        <v>0.0005257489999999963</v>
+        <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>-1.9329838095076e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2023,10 +1517,10 @@
         <v>0.003749147920927062</v>
       </c>
       <c r="B79" t="n">
-        <v>0.0005257489999999961</v>
+        <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>-1.95841780700112e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2034,10 +1528,10 @@
         <v>0.003797838153666374</v>
       </c>
       <c r="B80" t="n">
-        <v>0.000525748999999996</v>
+        <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>-1.983851804494641e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2045,10 +1539,10 @@
         <v>0.003846528386405687</v>
       </c>
       <c r="B81" t="n">
-        <v>0.000525748999999996</v>
+        <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>-2.009285801988162e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2056,10 +1550,10 @@
         <v>0.003895218619144999</v>
       </c>
       <c r="B82" t="n">
-        <v>0.0005257489999999959</v>
+        <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>-2.034719799481683e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2067,10 +1561,10 @@
         <v>0.003943908851884312</v>
       </c>
       <c r="B83" t="n">
-        <v>0.0005257489999999958</v>
+        <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>-2.060153796975204e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2078,10 +1572,10 @@
         <v>0.003992599084623624</v>
       </c>
       <c r="B84" t="n">
-        <v>0.0005257489999999957</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>-2.085587794468725e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2089,10 +1583,10 @@
         <v>0.004041289317362937</v>
       </c>
       <c r="B85" t="n">
-        <v>0.0005257489999999956</v>
+        <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>-2.111021791962246e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2100,10 +1594,10 @@
         <v>0.00408997955010225</v>
       </c>
       <c r="B86" t="n">
-        <v>0.0005257489999999955</v>
+        <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>-2.136455789455767e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2111,10 +1605,10 @@
         <v>0.004138669782841562</v>
       </c>
       <c r="B87" t="n">
-        <v>0.0005257489999999954</v>
+        <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>-2.161889786949287e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2122,10 +1616,10 @@
         <v>0.004187360015580874</v>
       </c>
       <c r="B88" t="n">
-        <v>0.0005257489999999953</v>
+        <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>-2.187323784442808e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -2133,10 +1627,10 @@
         <v>0.004236050248320187</v>
       </c>
       <c r="B89" t="n">
-        <v>0.0005257489999999952</v>
+        <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>-2.212757781936329e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -2144,10 +1638,10 @@
         <v>0.004284740481059499</v>
       </c>
       <c r="B90" t="n">
-        <v>0.0005257489999999951</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>-2.23819177942985e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2155,10 +1649,10 @@
         <v>0.004333430713798812</v>
       </c>
       <c r="B91" t="n">
-        <v>0.000525748999999995</v>
+        <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>-2.263625776923371e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2166,10 +1660,10 @@
         <v>0.004382120946538125</v>
       </c>
       <c r="B92" t="n">
-        <v>0.0005257489999999948</v>
+        <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>-2.289059774416893e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2177,10 +1671,10 @@
         <v>0.004430811179277437</v>
       </c>
       <c r="B93" t="n">
-        <v>0.0005257489999999947</v>
+        <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>-2.314493771910414e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2188,10 +1682,10 @@
         <v>0.004479501412016749</v>
       </c>
       <c r="B94" t="n">
-        <v>0.0005257489999999946</v>
+        <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>-2.339927769403934e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2199,10 +1693,10 @@
         <v>0.004528191644756062</v>
       </c>
       <c r="B95" t="n">
-        <v>0.0005257489999999945</v>
+        <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>-2.365361766897455e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2210,10 +1704,10 @@
         <v>0.004576881877495375</v>
       </c>
       <c r="B96" t="n">
-        <v>0.0005257489999999944</v>
+        <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>-2.390795764390976e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2221,10 +1715,10 @@
         <v>0.004625572110234687</v>
       </c>
       <c r="B97" t="n">
-        <v>0.0005257489999999943</v>
+        <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>-2.416229761884497e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2232,10 +1726,10 @@
         <v>0.004674262342973999</v>
       </c>
       <c r="B98" t="n">
-        <v>0.0005257489999999942</v>
+        <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>-2.441663759378018e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -2243,10 +1737,10 @@
         <v>0.004722952575713312</v>
       </c>
       <c r="B99" t="n">
-        <v>0.000525748999999994</v>
+        <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>-2.467097756871539e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -2254,10 +1748,10 @@
         <v>0.004771642808452625</v>
       </c>
       <c r="B100" t="n">
-        <v>0.0005257489999999939</v>
+        <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>-2.49253175436506e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -2265,10 +1759,10 @@
         <v>0.004820333041191937</v>
       </c>
       <c r="B101" t="n">
-        <v>0.0005257489999999938</v>
+        <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>-2.517965751858581e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -2276,10 +1770,10 @@
         <v>0.004869023273931249</v>
       </c>
       <c r="B102" t="n">
-        <v>0.0005257489999999937</v>
+        <v>0</v>
       </c>
       <c r="C102" t="n">
-        <v>-2.543399749352102e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -2287,10 +1781,10 @@
         <v>0.004917713506670562</v>
       </c>
       <c r="B103" t="n">
-        <v>0.0005257489999999935</v>
+        <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>-2.568833746845623e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -2298,10 +1792,10 @@
         <v>0.004966403739409875</v>
       </c>
       <c r="B104" t="n">
-        <v>0.0005257489999999934</v>
+        <v>0</v>
       </c>
       <c r="C104" t="n">
-        <v>-2.594267744339144e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -2309,10 +1803,10 @@
         <v>0.005015093972149187</v>
       </c>
       <c r="B105" t="n">
-        <v>0.0005257489999999933</v>
+        <v>0</v>
       </c>
       <c r="C105" t="n">
-        <v>-2.619701741832665e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -2320,10 +1814,10 @@
         <v>0.005063784204888499</v>
       </c>
       <c r="B106" t="n">
-        <v>0.0005257489999999931</v>
+        <v>0</v>
       </c>
       <c r="C106" t="n">
-        <v>-2.645135739326186e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -2331,10 +1825,10 @@
         <v>0.005112474437627812</v>
       </c>
       <c r="B107" t="n">
-        <v>0.000525748999999993</v>
+        <v>0</v>
       </c>
       <c r="C107" t="n">
-        <v>-2.670569736819708e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -2342,10 +1836,10 @@
         <v>0.005161164670367124</v>
       </c>
       <c r="B108" t="n">
-        <v>0.0005257489999999929</v>
+        <v>0</v>
       </c>
       <c r="C108" t="n">
-        <v>-2.696003734313228e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -2353,10 +1847,10 @@
         <v>0.005209854903106437</v>
       </c>
       <c r="B109" t="n">
-        <v>0.0005257489999999928</v>
+        <v>0</v>
       </c>
       <c r="C109" t="n">
-        <v>-2.721437731806749e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -2364,10 +1858,10 @@
         <v>0.005258545135845749</v>
       </c>
       <c r="B110" t="n">
-        <v>0.0005257489999999927</v>
+        <v>0</v>
       </c>
       <c r="C110" t="n">
-        <v>-2.74687172930027e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -2375,10 +1869,10 @@
         <v>0.005307235368585062</v>
       </c>
       <c r="B111" t="n">
-        <v>0.0005257489999999925</v>
+        <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>-2.772305726793792e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -2386,10 +1880,10 @@
         <v>0.005355925601324374</v>
       </c>
       <c r="B112" t="n">
-        <v>0.0005257489999999924</v>
+        <v>0</v>
       </c>
       <c r="C112" t="n">
-        <v>-2.797739724287313e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -2397,10 +1891,10 @@
         <v>0.005404615834063687</v>
       </c>
       <c r="B113" t="n">
-        <v>0.0005257489999999922</v>
+        <v>0</v>
       </c>
       <c r="C113" t="n">
-        <v>-2.823173721780834e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -2408,10 +1902,10 @@
         <v>0.005453306066803</v>
       </c>
       <c r="B114" t="n">
-        <v>0.0005257489999999921</v>
+        <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>-2.848607719274356e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -2419,10 +1913,10 @@
         <v>0.005501996299542311</v>
       </c>
       <c r="B115" t="n">
-        <v>0.0005257489999999919</v>
+        <v>0</v>
       </c>
       <c r="C115" t="n">
-        <v>-2.874041716767876e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -2430,10 +1924,10 @@
         <v>0.005550686532281624</v>
       </c>
       <c r="B116" t="n">
-        <v>0.0005257489999999918</v>
+        <v>0</v>
       </c>
       <c r="C116" t="n">
-        <v>-2.899475714261397e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -2441,10 +1935,10 @@
         <v>0.005599376765020937</v>
       </c>
       <c r="B117" t="n">
-        <v>0.0005257489999999917</v>
+        <v>0</v>
       </c>
       <c r="C117" t="n">
-        <v>-2.924909711754918e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -2452,10 +1946,10 @@
         <v>0.00564806699776025</v>
       </c>
       <c r="B118" t="n">
-        <v>0.0005257489999999915</v>
+        <v>0</v>
       </c>
       <c r="C118" t="n">
-        <v>-2.950343709248439e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -2463,10 +1957,10 @@
         <v>0.005696757230499561</v>
       </c>
       <c r="B119" t="n">
-        <v>0.0005257489999999914</v>
+        <v>0</v>
       </c>
       <c r="C119" t="n">
-        <v>-2.97577770674196e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -2474,10 +1968,10 @@
         <v>0.005745447463238874</v>
       </c>
       <c r="B120" t="n">
-        <v>0.0005257489999999913</v>
+        <v>0</v>
       </c>
       <c r="C120" t="n">
-        <v>-3.001211704235481e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -2485,10 +1979,10 @@
         <v>0.005794137695978187</v>
       </c>
       <c r="B121" t="n">
-        <v>0.0005257489999999911</v>
+        <v>0</v>
       </c>
       <c r="C121" t="n">
-        <v>-3.026645701729002e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -2496,10 +1990,10 @@
         <v>0.0058428279287175</v>
       </c>
       <c r="B122" t="n">
-        <v>0.0005257489999999909</v>
+        <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>-3.052079699222523e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -2507,10 +2001,10 @@
         <v>0.005891518161456812</v>
       </c>
       <c r="B123" t="n">
-        <v>0.0005257489999999908</v>
+        <v>0</v>
       </c>
       <c r="C123" t="n">
-        <v>-3.077513696716044e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -2518,10 +2012,10 @@
         <v>0.005940208394196124</v>
       </c>
       <c r="B124" t="n">
-        <v>0.0005257489999999906</v>
+        <v>0</v>
       </c>
       <c r="C124" t="n">
-        <v>-3.102947694209565e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -2529,10 +2023,10 @@
         <v>0.005988898626935437</v>
       </c>
       <c r="B125" t="n">
-        <v>0.0005257489999999905</v>
+        <v>0</v>
       </c>
       <c r="C125" t="n">
-        <v>-3.128381691703086e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -2540,10 +2034,10 @@
         <v>0.006037588859674749</v>
       </c>
       <c r="B126" t="n">
-        <v>0.0005257489999999903</v>
+        <v>0</v>
       </c>
       <c r="C126" t="n">
-        <v>-3.153815689196606e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -2551,10 +2045,10 @@
         <v>0.006086279092414062</v>
       </c>
       <c r="B127" t="n">
-        <v>0.0005257489999999902</v>
+        <v>0</v>
       </c>
       <c r="C127" t="n">
-        <v>-3.179249686690127e-15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2598,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -2609,10 +2103,10 @@
         <v>0.0001</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-5.223634405219401e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2620,10 +2114,10 @@
         <v>0.0002</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.04472688104388e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2631,10 +2125,10 @@
         <v>0.0003</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.56709032156582e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2642,10 +2136,10 @@
         <v>0.0004</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.08945376208776e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2653,10 +2147,10 @@
         <v>0.0005</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-2.6118172026097e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2664,10 +2158,10 @@
         <v>0.0006000000000000001</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>-3.13418064313164e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2675,10 +2169,10 @@
         <v>0.0007</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-3.65654408365358e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2686,10 +2180,10 @@
         <v>0.0008</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-4.17890752417552e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2697,10 +2191,10 @@
         <v>0.0009000000000000001</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.70127096469746e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2708,10 +2202,10 @@
         <v>0.001</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0005257489999999998</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>-5.2236344052194e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2719,10 +2213,10 @@
         <v>0.0011</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0005257489999999997</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>-5.74599784574134e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2730,10 +2224,10 @@
         <v>0.0012</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0005257489999999996</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>-6.26836128626328e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2741,10 +2235,10 @@
         <v>0.0013</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0005257489999999995</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>-6.790724726785219e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2752,10 +2246,10 @@
         <v>0.0014</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0005257489999999994</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>-7.313088167307159e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2763,10 +2257,10 @@
         <v>0.0015</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0005257489999999993</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>-7.835451607829098e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2774,10 +2268,10 @@
         <v>0.0016</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0005257489999999992</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>-8.357815048351037e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2785,10 +2279,10 @@
         <v>0.0017</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0005257489999999991</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>-8.880178488872976e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2796,10 +2290,10 @@
         <v>0.0018</v>
       </c>
       <c r="B20" t="n">
-        <v>0.000525748999999999</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>-9.402541929394914e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2807,10 +2301,10 @@
         <v>0.0019</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0005257489999999989</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>-9.924905369916852e-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2818,10 +2312,10 @@
         <v>0.002</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0005257489999999988</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.044726881043879e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2829,10 +2323,10 @@
         <v>0.0021</v>
       </c>
       <c r="B23" t="n">
-        <v>0.0005257489999999986</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>-1.096963225096073e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2840,10 +2334,10 @@
         <v>0.0022</v>
       </c>
       <c r="B24" t="n">
-        <v>0.0005257489999999985</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.149199569148267e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2851,10 +2345,10 @@
         <v>0.0023</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0005257489999999984</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>-1.20143591320046e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2862,10 +2356,10 @@
         <v>0.0024</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0005257489999999983</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.253672257252654e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -2873,10 +2367,10 @@
         <v>0.0025</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0005257489999999982</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>-1.305908601304848e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -2884,10 +2378,10 @@
         <v>0.0026</v>
       </c>
       <c r="B28" t="n">
-        <v>0.0005257489999999981</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.358144945357042e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2895,10 +2389,10 @@
         <v>0.0027</v>
       </c>
       <c r="B29" t="n">
-        <v>0.000525748999999998</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.410381289409235e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2906,10 +2400,10 @@
         <v>0.0028</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0005257489999999979</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.462617633461429e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2917,10 +2411,10 @@
         <v>0.0029</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0005257489999999978</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.514853977513623e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2928,10 +2422,10 @@
         <v>0.003</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0005257489999999977</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.567090321565817e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2939,10 +2433,10 @@
         <v>0.0031</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0005257489999999976</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.61932666561801e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2950,10 +2444,10 @@
         <v>0.0032</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0005257489999999973</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.671563009670204e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2961,10 +2455,10 @@
         <v>0.0033</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0005257489999999971</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.723799353722398e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2972,10 +2466,10 @@
         <v>0.0034</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0005257489999999969</v>
+        <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.776035697774591e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2983,10 +2477,10 @@
         <v>0.0035</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0005257489999999967</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.828272041826785e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2994,10 +2488,10 @@
         <v>0.0036</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0005257489999999965</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>-1.880508385878978e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -3005,10 +2499,10 @@
         <v>0.0037</v>
       </c>
       <c r="B39" t="n">
-        <v>0.0005257489999999963</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>-1.932744729931172e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -3016,10 +2510,10 @@
         <v>0.0038</v>
       </c>
       <c r="B40" t="n">
-        <v>0.000525748999999996</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.984981073983365e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -3027,10 +2521,10 @@
         <v>0.0039</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0005257489999999958</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>-2.037217418035559e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -3038,10 +2532,10 @@
         <v>0.004</v>
       </c>
       <c r="B42" t="n">
-        <v>0.0005257489999999956</v>
+        <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>-2.089453762087753e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -3049,10 +2543,10 @@
         <v>0.0041</v>
       </c>
       <c r="B43" t="n">
-        <v>0.0005257489999999954</v>
+        <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>-2.141690106139946e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -3060,10 +2554,10 @@
         <v>0.004200000000000001</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0005257489999999952</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>-2.193926450192139e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -3071,10 +2565,10 @@
         <v>0.0043</v>
       </c>
       <c r="B45" t="n">
-        <v>0.000525748999999995</v>
+        <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>-2.246162794244332e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -3082,10 +2576,10 @@
         <v>0.0044</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0005257489999999947</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>-2.298399138296526e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -3093,10 +2587,10 @@
         <v>0.004500000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0005257489999999945</v>
+        <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>-2.350635482348719e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -3104,10 +2598,10 @@
         <v>0.0046</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0005257489999999943</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>-2.402871826400912e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -3115,10 +2609,10 @@
         <v>0.0047</v>
       </c>
       <c r="B49" t="n">
-        <v>0.0005257489999999941</v>
+        <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>-2.455108170453105e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -3126,10 +2620,10 @@
         <v>0.0048</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0005257489999999939</v>
+        <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>-2.507344514505298e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -3137,10 +2631,10 @@
         <v>0.0049</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0005257489999999937</v>
+        <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>-2.559580858557492e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -3148,10 +2642,10 @@
         <v>0.005</v>
       </c>
       <c r="B52" t="n">
-        <v>0.0005257489999999934</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>-2.611817202609685e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -3159,10 +2653,10 @@
         <v>0.0051</v>
       </c>
       <c r="B53" t="n">
-        <v>0.0005257489999999932</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>-2.664053546661878e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -3170,10 +2664,10 @@
         <v>0.005200000000000001</v>
       </c>
       <c r="B54" t="n">
-        <v>0.000525748999999993</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>-2.716289890714071e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -3181,10 +2675,10 @@
         <v>0.0053</v>
       </c>
       <c r="B55" t="n">
-        <v>0.0005257489999999927</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>-2.768526234766264e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -3192,10 +2686,10 @@
         <v>0.0054</v>
       </c>
       <c r="B56" t="n">
-        <v>0.0005257489999999924</v>
+        <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>-2.820762578818458e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -3203,10 +2697,10 @@
         <v>0.005500000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>0.000525748999999992</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>-2.87299892287065e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -3214,10 +2708,10 @@
         <v>0.0056</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0005257489999999917</v>
+        <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>-2.925235266922843e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -3225,10 +2719,10 @@
         <v>0.0057</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0005257489999999914</v>
+        <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>-2.977471610975036e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -3236,10 +2730,10 @@
         <v>0.0058</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0005257489999999911</v>
+        <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>-3.029707955027229e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -3247,10 +2741,10 @@
         <v>0.0059</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0005257489999999907</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>-3.081944299079422e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -3258,10 +2752,10 @@
         <v>0.006</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0005257489999999904</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>-3.134180643131614e-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -3269,10 +2763,10 @@
         <v>0.0061</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0005257489999999901</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>-3.186416987183807e-15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3328,13 +2822,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0003504788812736815</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0001</v>
+        <v>0.0004057519394942708</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -3349,10 +2843,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0003504788812736812</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -3373,7 +2867,7 @@
         <v>302</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0003504788812736814</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0.0001</v>

</xml_diff>